<commit_message>
Sale Launch.xlsx: update location of projects within latest 2 years
</commit_message>
<xml_diff>
--- a/document/Sales Launch.xlsx
+++ b/document/Sales Launch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" tabRatio="713" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" tabRatio="713" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Flat type" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="177">
   <si>
     <t>Quarterly</t>
   </si>
@@ -191,13 +191,382 @@
   </si>
   <si>
     <t>No information provided</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>BTO</t>
+  </si>
+  <si>
+    <t>2017-Q2</t>
+  </si>
+  <si>
+    <t>Woodlands</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>https://www.google.com.sg/search?q=marsiling+grove&amp;tbm=isch&amp;source=iu&amp;pf=m&amp;ictx=1&amp;fir=HNshvIZyFwatEM%253A%252CTjNc0o0wYBf-xM%252C_&amp;usg=__8L3ti6gBwF1DTnI9qLREGN-b2SM%3D&amp;sa=X&amp;ved=0ahUKEwjahPW_7JrXAhXKQI8KHdheDQ8Q9QEIWjAJ#imgrc=HNshvIZyFwatEM:</t>
+  </si>
+  <si>
+    <t>https://www.google.com.sg/maps/@1.3502703,103.7454124,3a,75y,183.75h,81.63t/data=!3m7!1e1!3m5!1sZ2FFdBspX7R20Did4FXq2Q!2e0!6s%2F%2Fgeo0.ggpht.com%2Fcbk%3Fpanoid%3DZ2FFdBspX7R20Did4FXq2Q%26output%3Dthumbnail%26cb_client%3Dmaps_sv.tactile.gps%26thumb%3D2%26w%3D203%26h%3D100%26yaw%3D145.88089%26pitch%3D0%26thumbfov%3D100!7i13312!8i6656</t>
+  </si>
+  <si>
+    <t>https://www.google.com.sg/maps/@1.362219,103.7416521,3a,75y,132.43h,84.49t/data=!3m7!1e1!3m5!1spt5yoNghFG-njEDP0XBGuA!2e0!6s%2F%2Fgeo1.ggpht.com%2Fcbk%3Fpanoid%3Dpt5yoNghFG-njEDP0XBGuA%26output%3Dthumbnail%26cb_client%3Dmaps_sv.tactile.gps%26thumb%3D2%26w%3D203%26h%3D100%26yaw%3D264.11963%26pitch%3D0%26thumbfov%3D100!7i13312!8i6656</t>
+  </si>
+  <si>
+    <t>https://www.google.com.sg/maps/@1.3875883,103.9126596,3a,75y,228.18h,86.36t/data=!3m7!1e1!3m5!1sc3R5LpKO5yqlaXUrA_6PSQ!2e0!6s%2F%2Fgeo0.ggpht.com%2Fcbk%3Fpanoid%3Dc3R5LpKO5yqlaXUrA_6PSQ%26output%3Dthumbnail%26cb_client%3Dmaps_sv.tactile.gps%26thumb%3D2%26w%3D203%26h%3D100%26yaw%3D332.25784%26pitch%3D0%26thumbfov%3D100!7i13312!8i6656?hl=en</t>
+  </si>
+  <si>
+    <t>Marsiling Grove</t>
+  </si>
+  <si>
+    <t>103.77.4341</t>
+  </si>
+  <si>
+    <t>Woodlands Spring</t>
+  </si>
+  <si>
+    <t>https://www.renonation.sg/wp-content/uploads/Woodlands-Spring-Location-Map.jpg</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/static.streetsine/HDB_BTO/May2017/Yishun/BTO%20May_Yishun.jpg?20170523112019</t>
+  </si>
+  <si>
+    <t>Yishun</t>
+  </si>
+  <si>
+    <t>Forest Spring</t>
+  </si>
+  <si>
+    <t>Bidadari</t>
+  </si>
+  <si>
+    <t>Woodleigh Hillside</t>
+  </si>
+  <si>
+    <t>https://www.renonation.sg/wp-content/uploads/Woodleigh-Hillside-Site-Plan.jpg</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>The landmark is not shown on Google map, hence I make my best guess in the center</t>
+  </si>
+  <si>
+    <t>Geylang</t>
+  </si>
+  <si>
+    <t>Dakota Breeze</t>
+  </si>
+  <si>
+    <t>Pine Vista</t>
+  </si>
+  <si>
+    <t>https://www.renonation.sg/wp-content/uploads/2-GEYLANG-RIVER-VIEW-Dakota-Breeze-Site-Plan.jpg</t>
+  </si>
+  <si>
+    <t>Not shown on Google map</t>
+  </si>
+  <si>
+    <t>https://www.renonation.sg/wp-content/uploads/Intro-pic-for-dakota-and-pine.jpg</t>
+  </si>
+  <si>
+    <t>2017-Q1</t>
+  </si>
+  <si>
+    <t>Punggol</t>
+  </si>
+  <si>
+    <t>Clementi</t>
+  </si>
+  <si>
+    <t>Tampines</t>
+  </si>
+  <si>
+    <t>Northshore Cove</t>
+  </si>
+  <si>
+    <t>Waterway Sunrise II</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/static.streetsine/HDB_BTO/Feb2017/Punggol/Feb%202017%20BTO_punggol_2.jpg?20161130221127</t>
+  </si>
+  <si>
+    <t>Clementi NorthArc</t>
+  </si>
+  <si>
+    <t>Clementi Peaks</t>
+  </si>
+  <si>
+    <t>https://www.renonation.sg/wp-content/uploads/Clementi-Northarc-Site-map.jpg</t>
+  </si>
+  <si>
+    <t>http://esales.hdb.gov.sg/hdbvsf/eampu02p.nsf/0/17FEBBTOCL_images_1928/$file/map_02-02.jpg</t>
+  </si>
+  <si>
+    <t>Tampines GreenBloom</t>
+  </si>
+  <si>
+    <t>Tampines GreenFlora</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/static.streetsine/HDB_BTO/Feb2017/Tampines/Feb%2017%20BTO_Tampines_2.jpg?20161130221546</t>
+  </si>
+  <si>
+    <t>2016-Q4</t>
+  </si>
+  <si>
+    <t>Bedok</t>
+  </si>
+  <si>
+    <t>Kallang/Whampoa</t>
+  </si>
+  <si>
+    <t>Matilda Sundeck</t>
+  </si>
+  <si>
+    <t>Northshore Trio</t>
+  </si>
+  <si>
+    <t>Waterway Sunrise I</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2017_01/58895802cefdf_HDBMATILDASUNDECKcentralrubbishbins.png.1328bfd5c70034113fba399a795966da.png</t>
+  </si>
+  <si>
+    <t>Not shown on Google map. Might collapse with Verandah project</t>
+  </si>
+  <si>
+    <t>http://esales.hdb.gov.sg/hdbvsf/eampu11p.nsf/0/16NOVBTOPG_images_6429/$file/map_03-2.jpg</t>
+  </si>
+  <si>
+    <t>Not Shown on Google map</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2017_01/588be75acf198_waterwaysunriseIflyingstarstotal.png.fad0623892df5e6ffe8084dc1b0b5fa1.png</t>
+  </si>
+  <si>
+    <t>Bedok Beacon</t>
+  </si>
+  <si>
+    <t>Bedok North Vale</t>
+  </si>
+  <si>
+    <t>Bedok South Horizon</t>
+  </si>
+  <si>
+    <t>http://esales.hdb.gov.sg/hdbvsf/eampu11p.nsf/0/16NOVBTOBD_images_6429/$file/map_04.jpg</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2017_01/5886e5a883cda_HDBBedokNorthValeFlyingStars.png.46a21ddc8deffa8a92bbb960061f87b3.png</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2017_01/5886db7595924_BedokSouthHorizonTOTALFLYINGSTARS.png.d82bee1402983bd16a1ab7a8b32fab0a.png</t>
+  </si>
+  <si>
+    <t>Woodleigh Glen</t>
+  </si>
+  <si>
+    <t>Woodleigh Village</t>
+  </si>
+  <si>
+    <t>https://www.renonation.sg/wp-content/uploads/woodleigh-glen-sitemap.jpg</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2017_01/588c70181eb89_HDBWoodleighVillageTOTALSMALL.png.be4e6904d3107a4ec5916216520a9edc.png</t>
+  </si>
+  <si>
+    <t>My guess based on guessed location of Woodleign Glen</t>
+  </si>
+  <si>
+    <t>Kalang Residences</t>
+  </si>
+  <si>
+    <t>http://www.hdb.gov.sg/cs/infoweb/img/corporate-pr-21112016-kallang-residences-map.jpg</t>
+  </si>
+  <si>
+    <t>2016-Q3</t>
+  </si>
+  <si>
+    <t>Hougang</t>
+  </si>
+  <si>
+    <t>Sembawang</t>
+  </si>
+  <si>
+    <t>Buangkok Woods</t>
+  </si>
+  <si>
+    <t>EastDelta @Canberra</t>
+  </si>
+  <si>
+    <t>Valley Spring</t>
+  </si>
+  <si>
+    <t>Tampines GreenView</t>
+  </si>
+  <si>
+    <t>Tampines GreenVerge</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2016_08/57b971b3e9966_buangkokwoodsprecinctpavilion.png.9e38cf5084f37f1a35a2cedf5f492121.png</t>
+  </si>
+  <si>
+    <t>Not sure about this one. Information of this quarter is from http://www.hdb.gov.sg/cs/infoweb/press-release/hdb-launches-4,841-flats-in-august-2016-bto-exercise</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2016_08/57bbb1a25a93f_eastdeltaatcanberraflyingstarsworking1.png.bdb730953333401c7298c3e82068534f.png</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2016_08/57b66a27aa9a8_TotalFlyingStars-ValleySpringYishun.png.09b72374d40bdaf0b80cb6d97450982f.png</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2016_08/57b6b76e74685_Totaltampinesgreenviewflyingstars.png.6bb37cec2de85d998055a2d42edaac3c.png</t>
+  </si>
+  <si>
+    <t>http://www.hdb.gov.sg/cs/infoweb/img/corp_pr_17082016_location-map_tampines.jpg</t>
+  </si>
+  <si>
+    <t>Information of this quarter: http://www.hdb.gov.sg/cs/infoweb/press-release/hdb-launches-8940-flats-in-may-2016-bto-cum-sbf-exercise</t>
+  </si>
+  <si>
+    <t>2016-Q2</t>
+  </si>
+  <si>
+    <t>Sewbawang</t>
+  </si>
+  <si>
+    <t>EastCreek @Canberra</t>
+  </si>
+  <si>
+    <t>Bukit Panjang</t>
+  </si>
+  <si>
+    <t>Senja Valley</t>
+  </si>
+  <si>
+    <t>Senja Heights</t>
+  </si>
+  <si>
+    <t>Senja Ridges</t>
+  </si>
+  <si>
+    <t>Ang Mo Kio Court</t>
+  </si>
+  <si>
+    <t>Bedok North Woods</t>
+  </si>
+  <si>
+    <t>Ang Mo Kio</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2016_08/57c5621b50fc7_HDBEASTCREEKnWATERCLASSICS.png.afee57b9af202b99f08e6047db248436.png</t>
+  </si>
+  <si>
+    <t>http://www.hdb.gov.sg/cs/infoweb/img/corporate-pr-senja-heights-senja-ridges-senja-valley_location-ma.jpg</t>
+  </si>
+  <si>
+    <t>https://www.propertyhunt.sg/wp-content/uploads/2016/06/Amk-court-1.png</t>
+  </si>
+  <si>
+    <t>http://www.hdb.gov.sg/cs/infoweb/img/corporate-pr-bedok-north-woods-location-map-24052016.jpg</t>
+  </si>
+  <si>
+    <t>2016-Q1</t>
+  </si>
+  <si>
+    <t>West Plains</t>
+  </si>
+  <si>
+    <t>Anchorvale Plains</t>
+  </si>
+  <si>
+    <t>Alkaff Oasis</t>
+  </si>
+  <si>
+    <t>https://static.straitstimes.com.sg/sites/default/files/bb1.jpg</t>
+  </si>
+  <si>
+    <t>Toa Payoh</t>
+  </si>
+  <si>
+    <t>https://static.straitstimes.com.sg/sites/default/files/sengkang1.jpg</t>
+  </si>
+  <si>
+    <t>https://static.straitstimes.com.sg/sites/default/files/alkaff2.jpg</t>
+  </si>
+  <si>
+    <t>2015-Q4</t>
+  </si>
+  <si>
+    <t>Information of this quarter: http://www.hdb.gov.sg/cs/infoweb/press-releases/hdb-launches-bumper-crop-of-12411-flats</t>
+  </si>
+  <si>
+    <t>Alkaff CourtView</t>
+  </si>
+  <si>
+    <t>Alkaff LakeView</t>
+  </si>
+  <si>
+    <t>Alkaff Vista</t>
+  </si>
+  <si>
+    <t>Waterfront I &amp; II @Northshore</t>
+  </si>
+  <si>
+    <t>Northshore StraitsView</t>
+  </si>
+  <si>
+    <t>Choa Chu Kang</t>
+  </si>
+  <si>
+    <t>Teck Whye Vista</t>
+  </si>
+  <si>
+    <t>Fernvale Woods</t>
+  </si>
+  <si>
+    <t>West Quarry</t>
+  </si>
+  <si>
+    <t>Hougang RiverCourt</t>
+  </si>
+  <si>
+    <t>https://www.homerenoguru.sg/wp-content/uploads/usercontent/launches/140-teck-whye-vista/teck-whye-vista-location-map.jpg</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2016_08/hdb_fernvale_woods_poison_arrows.png.bdc57cd428fbdb5165187532f540ec98.png</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/y2l7Q1y.png?1</t>
+  </si>
+  <si>
+    <t>Road name does not match. Yet it looks right though</t>
+  </si>
+  <si>
+    <t>https://www.homerenoguru.sg/wp-content/uploads/usercontent/launches/137-hougang-rivercourt/hougang-rivercourt-location-map.jpg</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2016_08/waterfront_1_and_2_-_precinct_pavilion.png.ef05620270be485c689c281a606fa5c6.png</t>
+  </si>
+  <si>
+    <t>https://www.geomancy.net/forums/uploads/monthly_2016_08/hdb_straits_view_total.png.313390a18fc8fac24a998b904c4023bb.png</t>
+  </si>
+  <si>
+    <t>https://www.homerenoguru.sg/wp-content/uploads/usercontent/launches/141-alkaff-courtview/alkaff-courtview-location-map.jpg</t>
+  </si>
+  <si>
+    <t>https://www.renonation.sg/wp-content/uploads/Alkaff-Vista-siteplan.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +579,14 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -229,14 +606,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -323,14 +703,17 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:H48" totalsRowShown="0">
+  <autoFilter ref="A1:H48"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Quarterly"/>
+    <tableColumn id="6" name="Type"/>
     <tableColumn id="2" name="Town"/>
     <tableColumn id="3" name="Contract"/>
     <tableColumn id="4" name="Longitude"/>
     <tableColumn id="5" name="Latitude"/>
+    <tableColumn id="8" name="Note"/>
+    <tableColumn id="7" name="Map"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1093,7 +1476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1176,7 +1559,7 @@
         <v>32</v>
       </c>
       <c r="K2">
-        <f>F2/J2</f>
+        <f t="shared" ref="K2:K22" si="0">F2/J2</f>
         <v>0.84375</v>
       </c>
     </row>
@@ -1213,7 +1596,7 @@
         <v>114</v>
       </c>
       <c r="K3">
-        <f>F3/J3</f>
+        <f t="shared" si="0"/>
         <v>0.84210526315789469</v>
       </c>
     </row>
@@ -1250,7 +1633,7 @@
         <v>149</v>
       </c>
       <c r="K4">
-        <f>F4/J4</f>
+        <f t="shared" si="0"/>
         <v>0.84563758389261745</v>
       </c>
     </row>
@@ -1287,7 +1670,7 @@
         <v>173</v>
       </c>
       <c r="K5">
-        <f>F5/J5</f>
+        <f t="shared" si="0"/>
         <v>0.84393063583815031</v>
       </c>
     </row>
@@ -1320,11 +1703,11 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J22" si="0">SUM(G6, H6,I6)</f>
+        <f t="shared" ref="J6:J22" si="1">SUM(G6, H6,I6)</f>
         <v>141</v>
       </c>
       <c r="K6">
-        <f>F6/J6</f>
+        <f t="shared" si="0"/>
         <v>0.85106382978723405</v>
       </c>
     </row>
@@ -1357,11 +1740,11 @@
         <v>14</v>
       </c>
       <c r="J7">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="0"/>
-        <v>133</v>
-      </c>
-      <c r="K7">
-        <f>F7/J7</f>
         <v>0.84210526315789469</v>
       </c>
     </row>
@@ -1394,11 +1777,11 @@
         <v>9</v>
       </c>
       <c r="J8">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="0"/>
-        <v>94</v>
-      </c>
-      <c r="K8">
-        <f>F8/J8</f>
         <v>0.85106382978723405</v>
       </c>
     </row>
@@ -1431,11 +1814,11 @@
         <v>6</v>
       </c>
       <c r="J9">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="K9">
-        <f>F9/J9</f>
         <v>0.8571428571428571</v>
       </c>
     </row>
@@ -1468,11 +1851,11 @@
         <v>4</v>
       </c>
       <c r="J10">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="K10">
-        <f>F10/J10</f>
         <v>0.84210526315789469</v>
       </c>
     </row>
@@ -1505,11 +1888,11 @@
         <v>3</v>
       </c>
       <c r="J11">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="K11">
-        <f>F11/J11</f>
         <v>0.82352941176470584</v>
       </c>
     </row>
@@ -1542,11 +1925,11 @@
         <v>4</v>
       </c>
       <c r="J12">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="K12">
-        <f>F12/J12</f>
         <v>0.81081081081081086</v>
       </c>
     </row>
@@ -1579,11 +1962,11 @@
         <v>3</v>
       </c>
       <c r="J13">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="K13">
-        <f>F13/J13</f>
         <v>0.84848484848484851</v>
       </c>
     </row>
@@ -1616,11 +1999,11 @@
         <v>6</v>
       </c>
       <c r="J14">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="K14">
-        <f>F14/J14</f>
         <v>0.85185185185185186</v>
       </c>
     </row>
@@ -1653,11 +2036,11 @@
         <v>13</v>
       </c>
       <c r="J15">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-      <c r="K15">
-        <f>F15/J15</f>
         <v>0.84677419354838712</v>
       </c>
     </row>
@@ -1690,11 +2073,11 @@
         <v>4</v>
       </c>
       <c r="J16">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="K16">
-        <f>F16/J16</f>
         <v>0.84210526315789469</v>
       </c>
     </row>
@@ -1727,11 +2110,11 @@
         <v>4</v>
       </c>
       <c r="J17">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="K17">
-        <f>F17/J17</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -1764,11 +2147,11 @@
         <v>5</v>
       </c>
       <c r="J18">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="K18">
-        <f>F18/J18</f>
         <v>0.84313725490196079</v>
       </c>
     </row>
@@ -1801,11 +2184,11 @@
         <v>5</v>
       </c>
       <c r="J19">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="K19">
-        <f>F19/J19</f>
         <v>0.84</v>
       </c>
     </row>
@@ -1838,11 +2221,11 @@
         <v>5</v>
       </c>
       <c r="J20">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="K20">
-        <f>F20/J20</f>
         <v>0.875</v>
       </c>
     </row>
@@ -1875,11 +2258,11 @@
         <v>12</v>
       </c>
       <c r="J21">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="0"/>
-        <v>111</v>
-      </c>
-      <c r="K21">
-        <f>F21/J21</f>
         <v>0.84684684684684686</v>
       </c>
     </row>
@@ -1912,11 +2295,11 @@
         <v>11</v>
       </c>
       <c r="J22">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="K22">
-        <f>F22/J22</f>
         <v>0.84</v>
       </c>
     </row>
@@ -2266,93 +2649,1215 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.35022</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>103.745318</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.3621209999999999</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>103.74143100000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.3874759999999999</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>103.91282</v>
       </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5">
+        <v>1.4374709999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6">
+        <v>1.446501</v>
+      </c>
+      <c r="F6">
+        <v>103.799753</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7">
+        <v>1.4258439999999999</v>
+      </c>
+      <c r="F7">
+        <v>103.85252300000001</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8">
+        <v>1.3423609999999999</v>
+      </c>
+      <c r="F8">
+        <v>103.874274</v>
+      </c>
+      <c r="G8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>1.309895</v>
+      </c>
+      <c r="F9">
+        <v>103.888105</v>
+      </c>
+      <c r="G9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10">
+        <v>1.3096479999999999</v>
+      </c>
+      <c r="F10">
+        <v>103.885718</v>
+      </c>
+      <c r="G10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <v>1.419826</v>
+      </c>
+      <c r="F11">
+        <v>103.906594</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12">
+        <v>1.397653</v>
+      </c>
+      <c r="F12">
+        <v>103.920834</v>
+      </c>
+      <c r="G12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13">
+        <v>1.3224959999999999</v>
+      </c>
+      <c r="F13">
+        <v>103.76343199999999</v>
+      </c>
+      <c r="H13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14">
+        <v>1.310033</v>
+      </c>
+      <c r="F14">
+        <v>103.767605</v>
+      </c>
+      <c r="H14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15">
+        <v>1.353442</v>
+      </c>
+      <c r="F15">
+        <v>103.930182</v>
+      </c>
+      <c r="H15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16">
+        <v>1.3541179999999999</v>
+      </c>
+      <c r="F16">
+        <v>103.930632</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17">
+        <v>1.4030560000000001</v>
+      </c>
+      <c r="F17">
+        <v>103.893292</v>
+      </c>
+      <c r="G17" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18">
+        <v>1.417945</v>
+      </c>
+      <c r="F18">
+        <v>103.905901</v>
+      </c>
+      <c r="G18" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>1.3989279999999999</v>
+      </c>
+      <c r="F19">
+        <v>103.921026</v>
+      </c>
+      <c r="G19" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20">
+        <v>1.324578</v>
+      </c>
+      <c r="F20">
+        <v>103.927797</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21">
+        <v>1.329966</v>
+      </c>
+      <c r="F21">
+        <v>103.92563800000001</v>
+      </c>
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22">
+        <v>1.3179160000000001</v>
+      </c>
+      <c r="F22">
+        <v>103.947209</v>
+      </c>
+      <c r="G22" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23">
+        <v>1.341952</v>
+      </c>
+      <c r="F23">
+        <v>103.87165400000001</v>
+      </c>
+      <c r="G23" t="s">
+        <v>79</v>
+      </c>
+      <c r="H23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24">
+        <v>1.3406439999999999</v>
+      </c>
+      <c r="F24">
+        <v>103.87164300000001</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25">
+        <v>1.3116570000000001</v>
+      </c>
+      <c r="F25">
+        <v>103.872784</v>
+      </c>
+      <c r="H25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26">
+        <v>1.38107</v>
+      </c>
+      <c r="F26">
+        <v>103.881237</v>
+      </c>
+      <c r="G26" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27">
+        <v>1.445864</v>
+      </c>
+      <c r="F27">
+        <v>103.835064</v>
+      </c>
+      <c r="H27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28">
+        <v>1.4293039999999999</v>
+      </c>
+      <c r="F28">
+        <v>103.85086200000001</v>
+      </c>
+      <c r="G28" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29">
+        <v>1.3657349999999999</v>
+      </c>
+      <c r="F29">
+        <v>103.935441</v>
+      </c>
+      <c r="G29" t="s">
+        <v>171</v>
+      </c>
+      <c r="H29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30">
+        <v>1.3617319999999999</v>
+      </c>
+      <c r="F30">
+        <v>103.94006899999999</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31">
+        <v>1.4514020000000001</v>
+      </c>
+      <c r="F31">
+        <v>103.831208</v>
+      </c>
+      <c r="G31" t="s">
+        <v>133</v>
+      </c>
+      <c r="H31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32">
+        <v>1.38767</v>
+      </c>
+      <c r="F32">
+        <v>103.763017</v>
+      </c>
+      <c r="G32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33">
+        <v>1.3873260000000001</v>
+      </c>
+      <c r="F33">
+        <v>103.76218799999999</v>
+      </c>
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34">
+        <v>1.3886780000000001</v>
+      </c>
+      <c r="F34">
+        <v>103.761563</v>
+      </c>
+      <c r="G34" t="s">
+        <v>79</v>
+      </c>
+      <c r="H34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35">
+        <v>1.3678920000000001</v>
+      </c>
+      <c r="F35">
+        <v>103.840058</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36">
+        <v>1.330408</v>
+      </c>
+      <c r="F36">
+        <v>103.93249299999999</v>
+      </c>
+      <c r="H36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37">
+        <v>1.356976</v>
+      </c>
+      <c r="F37">
+        <v>103.742814</v>
+      </c>
+      <c r="G37" t="s">
+        <v>79</v>
+      </c>
+      <c r="H37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38">
+        <v>1.393551</v>
+      </c>
+      <c r="F38">
+        <v>103.885017</v>
+      </c>
+      <c r="G38" t="s">
+        <v>79</v>
+      </c>
+      <c r="H38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39">
+        <v>1.334657</v>
+      </c>
+      <c r="F39">
+        <v>103.87262800000001</v>
+      </c>
+      <c r="G39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" t="s">
+        <v>164</v>
+      </c>
+      <c r="E40">
+        <v>1.379089</v>
+      </c>
+      <c r="F40">
+        <v>103.75862100000001</v>
+      </c>
+      <c r="G40" t="s">
+        <v>157</v>
+      </c>
+      <c r="H40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>165</v>
+      </c>
+      <c r="E41">
+        <v>1.3921289999999999</v>
+      </c>
+      <c r="F41">
+        <v>103.870385</v>
+      </c>
+      <c r="G41" t="s">
+        <v>79</v>
+      </c>
+      <c r="H41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42">
+        <v>1.353844</v>
+      </c>
+      <c r="F42">
+        <v>103.739622</v>
+      </c>
+      <c r="G42" t="s">
+        <v>79</v>
+      </c>
+      <c r="H42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43">
+        <v>1.362646</v>
+      </c>
+      <c r="F43">
+        <v>103.894946</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44">
+        <v>1.4177599999999999</v>
+      </c>
+      <c r="F44">
+        <v>103.901758</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45">
+        <v>1.419303</v>
+      </c>
+      <c r="F45">
+        <v>103.904578</v>
+      </c>
+      <c r="H45" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46">
+        <v>1.336476</v>
+      </c>
+      <c r="F46">
+        <v>103.871205</v>
+      </c>
+      <c r="H46" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" t="s">
+        <v>159</v>
+      </c>
+      <c r="E47">
+        <v>1.336905</v>
+      </c>
+      <c r="F47">
+        <v>103.872535</v>
+      </c>
+      <c r="H47" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" t="s">
+        <v>160</v>
+      </c>
+      <c r="E48">
+        <v>1.3334490000000001</v>
+      </c>
+      <c r="F48">
+        <v>103.87011699999999</v>
+      </c>
+      <c r="H48" t="s">
+        <v>176</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2"/>
+    <hyperlink ref="H16" r:id="rId1"/>
+    <hyperlink ref="H20" r:id="rId2"/>
+    <hyperlink ref="H24" r:id="rId3"/>
+    <hyperlink ref="H30" r:id="rId4"/>
+    <hyperlink ref="H35" r:id="rId5"/>
+    <hyperlink ref="H43" r:id="rId6"/>
+    <hyperlink ref="H44" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add number of blocks per project for simulation
</commit_message>
<xml_diff>
--- a/document/Sales Launch.xlsx
+++ b/document/Sales Launch.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="243">
   <si>
     <t>Quarterly</t>
   </si>
@@ -740,6 +740,24 @@
   </si>
   <si>
     <t>Exclude 48 units of 3Gen flats:422</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -859,9 +877,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table47" displayName="Table47" ref="A1:K142" totalsRowShown="0">
-  <autoFilter ref="A1:K142"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table47" displayName="Table47" ref="A1:L142" totalsRowShown="0">
+  <autoFilter ref="A1:L142"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="Quarterly"/>
     <tableColumn id="2" name="Town"/>
     <tableColumn id="3" name="Flat Type"/>
@@ -877,6 +895,7 @@
     <tableColumn id="11" name="Ratio">
       <calculatedColumnFormula>F2/J2</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="12" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1686,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P141"/>
+  <dimension ref="A1:T141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="L126" sqref="L126"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,7 +1722,7 @@
     <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1737,8 +1756,11 @@
       <c r="K1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1778,7 +1800,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1815,7 +1837,7 @@
         <v>0.84210526315789469</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1851,8 +1873,14 @@
         <f t="shared" si="0"/>
         <v>0.84563758389261745</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1888,8 +1916,14 @@
         <f t="shared" si="0"/>
         <v>0.84393063583815031</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1925,8 +1959,17 @@
         <f t="shared" si="0"/>
         <v>0.85106382978723405</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1963,7 +2006,7 @@
         <v>0.84210526315789469</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2000,7 +2043,7 @@
         <v>0.85106382978723405</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2037,7 +2080,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2074,7 +2117,7 @@
         <v>0.84210526315789469</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2111,7 +2154,7 @@
         <v>0.82352941176470584</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2148,7 +2191,7 @@
         <v>0.81081081081081086</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2185,7 +2228,7 @@
         <v>0.84848484848484851</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2222,7 +2265,7 @@
         <v>0.85185185185185186</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2259,7 +2302,7 @@
         <v>0.84677419354838712</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2296,7 +2339,7 @@
         <v>0.84210526315789469</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2333,7 +2376,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2370,7 +2413,7 @@
         <v>0.84313725490196079</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2407,7 +2450,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2444,7 +2487,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2481,7 +2524,7 @@
         <v>0.84684684684684686</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -2518,7 +2561,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2546,8 +2589,29 @@
       <c r="I23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>238</v>
+      </c>
+      <c r="O23">
+        <v>170</v>
+      </c>
+      <c r="P23">
+        <v>171</v>
+      </c>
+      <c r="Q23">
+        <v>172</v>
+      </c>
+      <c r="R23">
+        <v>173</v>
+      </c>
+      <c r="S23">
+        <v>174</v>
+      </c>
+      <c r="T23">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2576,15 +2640,39 @@
         <v>21</v>
       </c>
       <c r="J24">
-        <f>SUM(G24, H24,I24)</f>
+        <f t="shared" ref="J24:J55" si="2">SUM(G24, H24,I24)</f>
         <v>207</v>
       </c>
       <c r="K24">
-        <f>F24/J24</f>
+        <f t="shared" ref="K24:K55" si="3">F24/J24</f>
         <v>0.84057971014492749</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>238</v>
+      </c>
+      <c r="N24" t="s">
+        <v>239</v>
+      </c>
+      <c r="O24" t="s">
+        <v>238</v>
+      </c>
+      <c r="P24" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>238</v>
+      </c>
+      <c r="R24" t="s">
+        <v>238</v>
+      </c>
+      <c r="S24" t="s">
+        <v>238</v>
+      </c>
+      <c r="T24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2613,15 +2701,39 @@
         <v>16</v>
       </c>
       <c r="J25">
-        <f>SUM(G25, H25,I25)</f>
+        <f t="shared" si="2"/>
         <v>153</v>
       </c>
       <c r="K25">
-        <f>F25/J25</f>
+        <f t="shared" si="3"/>
         <v>0.83660130718954251</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>238</v>
+      </c>
+      <c r="N25" t="s">
+        <v>237</v>
+      </c>
+      <c r="O25" t="s">
+        <v>238</v>
+      </c>
+      <c r="P25" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>238</v>
+      </c>
+      <c r="R25" t="s">
+        <v>238</v>
+      </c>
+      <c r="S25" t="s">
+        <v>238</v>
+      </c>
+      <c r="T25" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2650,15 +2762,27 @@
         <v>17</v>
       </c>
       <c r="J26">
-        <f>SUM(G26, H26,I26)</f>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="K26">
-        <f>F26/J26</f>
+        <f t="shared" si="3"/>
         <v>0.84023668639053251</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>238</v>
+      </c>
+      <c r="N26" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>238</v>
+      </c>
+      <c r="R26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2687,15 +2811,27 @@
         <v>8</v>
       </c>
       <c r="J27">
-        <f>SUM(G27, H27,I27)</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="K27">
-        <f>F27/J27</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>238</v>
+      </c>
+      <c r="N27" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>238</v>
+      </c>
+      <c r="R27" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2724,15 +2860,18 @@
         <v>8</v>
       </c>
       <c r="J28">
-        <f>SUM(G28, H28,I28)</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="K28">
-        <f>F28/J28</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2761,15 +2900,18 @@
         <v>17</v>
       </c>
       <c r="J29">
-        <f>SUM(G29, H29,I29)</f>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="K29">
-        <f>F29/J29</f>
+        <f t="shared" si="3"/>
         <v>0.84023668639053251</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2798,15 +2940,18 @@
         <v>16</v>
       </c>
       <c r="J30">
-        <f>SUM(G30, H30,I30)</f>
+        <f t="shared" si="2"/>
         <v>153</v>
       </c>
       <c r="K30">
-        <f>F30/J30</f>
+        <f t="shared" si="3"/>
         <v>0.83660130718954251</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -2835,15 +2980,18 @@
         <v>21</v>
       </c>
       <c r="J31">
-        <f>SUM(G31, H31,I31)</f>
+        <f t="shared" si="2"/>
         <v>207</v>
       </c>
       <c r="K31">
-        <f>F31/J31</f>
+        <f t="shared" si="3"/>
         <v>0.84057971014492749</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -2872,15 +3020,18 @@
         <v>4</v>
       </c>
       <c r="J32">
-        <f>SUM(G32, H32,I32)</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="K32">
-        <f>F32/J32</f>
+        <f t="shared" si="3"/>
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2909,15 +3060,18 @@
         <v>3</v>
       </c>
       <c r="J33">
-        <f>SUM(G33, H33,I33)</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="K33">
-        <f>F33/J33</f>
+        <f t="shared" si="3"/>
         <v>0.84615384615384615</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2946,15 +3100,18 @@
         <v>4</v>
       </c>
       <c r="J34">
-        <f>SUM(G34, H34,I34)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K34">
-        <f>F34/J34</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2983,15 +3140,18 @@
         <v>4</v>
       </c>
       <c r="J35">
-        <f>SUM(G35, H35,I35)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K35">
-        <f>F35/J35</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -3020,15 +3180,18 @@
         <v>4</v>
       </c>
       <c r="J36">
-        <f>SUM(G36, H36,I36)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K36">
-        <f>F36/J36</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -3057,15 +3220,18 @@
         <v>4</v>
       </c>
       <c r="J37">
-        <f>SUM(G37, H37,I37)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K37">
-        <f>F37/J37</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -3094,15 +3260,18 @@
         <v>3</v>
       </c>
       <c r="J38">
-        <f>SUM(G38, H38,I38)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="K38">
-        <f>F38/J38</f>
+        <f t="shared" si="3"/>
         <v>0.8571428571428571</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -3131,15 +3300,18 @@
         <v>7</v>
       </c>
       <c r="J39">
-        <f>SUM(G39, H39,I39)</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="K39">
-        <f>F39/J39</f>
+        <f t="shared" si="3"/>
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -3168,15 +3340,18 @@
         <v>9</v>
       </c>
       <c r="J40">
-        <f>SUM(G40, H40,I40)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="K40">
-        <f>F40/J40</f>
+        <f t="shared" si="3"/>
         <v>0.85882352941176465</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -3205,15 +3380,18 @@
         <v>7</v>
       </c>
       <c r="J41">
-        <f>SUM(G41, H41,I41)</f>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="K41">
-        <f>F41/J41</f>
+        <f t="shared" si="3"/>
         <v>0.828125</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -3242,24 +3420,18 @@
         <v>8</v>
       </c>
       <c r="J42">
-        <f>SUM(G42, H42,I42)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="K42">
-        <f>F42/J42</f>
+        <f t="shared" si="3"/>
         <v>0.82666666666666666</v>
       </c>
-      <c r="M42" t="s">
-        <v>40</v>
-      </c>
-      <c r="N42" t="s">
-        <v>41</v>
-      </c>
-      <c r="O42" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -3288,27 +3460,27 @@
         <v>4</v>
       </c>
       <c r="J43">
-        <f>SUM(G43, H43,I43)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K43">
-        <f>F43/J43</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
       <c r="L43" t="s">
-        <v>199</v>
-      </c>
-      <c r="M43">
-        <v>84</v>
-      </c>
-      <c r="N43">
-        <v>22</v>
-      </c>
-      <c r="O43">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>40</v>
+      </c>
+      <c r="R43" t="s">
+        <v>41</v>
+      </c>
+      <c r="S43" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -3337,27 +3509,30 @@
         <v>8</v>
       </c>
       <c r="J44">
-        <f>SUM(G44, H44,I44)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="K44">
-        <f>F44/J44</f>
+        <f t="shared" si="3"/>
         <v>0.83783783783783783</v>
       </c>
       <c r="L44" t="s">
-        <v>201</v>
-      </c>
-      <c r="M44">
-        <v>87</v>
-      </c>
-      <c r="N44">
-        <v>25</v>
-      </c>
-      <c r="O44">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="P44" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q44">
+        <v>84</v>
+      </c>
+      <c r="R44">
+        <v>22</v>
+      </c>
+      <c r="S44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -3386,15 +3561,30 @@
         <v>8</v>
       </c>
       <c r="J45">
-        <f>SUM(G45, H45,I45)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="K45">
-        <f>F45/J45</f>
+        <f t="shared" si="3"/>
         <v>0.83783783783783783</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>238</v>
+      </c>
+      <c r="P45" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q45">
+        <v>87</v>
+      </c>
+      <c r="R45">
+        <v>25</v>
+      </c>
+      <c r="S45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -3423,15 +3613,18 @@
         <v>4</v>
       </c>
       <c r="J46">
-        <f>SUM(G46, H46,I46)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K46">
-        <f>F46/J46</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -3460,27 +3653,18 @@
         <v>9</v>
       </c>
       <c r="J47">
-        <f>SUM(G47, H47,I47)</f>
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="K47">
-        <f>F47/J47</f>
+        <f t="shared" si="3"/>
         <v>0.84042553191489366</v>
       </c>
-      <c r="L47">
-        <v>81</v>
-      </c>
-      <c r="M47">
-        <v>0.22222</v>
-      </c>
-      <c r="N47">
-        <v>0.83950599999999997</v>
-      </c>
-      <c r="O47">
-        <v>0.123457</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L47" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -3509,27 +3693,30 @@
         <v>7</v>
       </c>
       <c r="J48">
-        <f>SUM(G48, H48,I48)</f>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="K48">
-        <f>F48/J48</f>
+        <f t="shared" si="3"/>
         <v>0.828125</v>
       </c>
-      <c r="L48">
-        <v>141</v>
-      </c>
-      <c r="M48">
-        <v>0.219858</v>
-      </c>
-      <c r="N48">
+      <c r="L48" t="s">
+        <v>238</v>
+      </c>
+      <c r="P48">
+        <v>81</v>
+      </c>
+      <c r="Q48">
+        <v>0.22222</v>
+      </c>
+      <c r="R48">
         <v>0.83950599999999997</v>
       </c>
-      <c r="O48">
+      <c r="S48">
         <v>0.123457</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -3558,27 +3745,30 @@
         <v>8</v>
       </c>
       <c r="J49">
-        <f>SUM(G49, H49,I49)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="K49">
-        <f>F49/J49</f>
+        <f t="shared" si="3"/>
         <v>0.82666666666666666</v>
       </c>
-      <c r="L49">
-        <v>62</v>
-      </c>
-      <c r="M49">
-        <v>0.22580600000000001</v>
-      </c>
-      <c r="N49">
+      <c r="L49" t="s">
+        <v>238</v>
+      </c>
+      <c r="P49">
+        <v>141</v>
+      </c>
+      <c r="Q49">
+        <v>0.219858</v>
+      </c>
+      <c r="R49">
         <v>0.83950599999999997</v>
       </c>
-      <c r="O49">
+      <c r="S49">
         <v>0.123457</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -3607,27 +3797,30 @@
         <v>7</v>
       </c>
       <c r="J50">
-        <f>SUM(G50, H50,I50)</f>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="K50">
-        <f>F50/J50</f>
+        <f t="shared" si="3"/>
         <v>0.828125</v>
       </c>
-      <c r="L50">
-        <v>174</v>
-      </c>
-      <c r="M50">
-        <v>0.224138</v>
-      </c>
-      <c r="N50">
+      <c r="L50" t="s">
+        <v>238</v>
+      </c>
+      <c r="P50">
+        <v>62</v>
+      </c>
+      <c r="Q50">
+        <v>0.22580600000000001</v>
+      </c>
+      <c r="R50">
         <v>0.83950599999999997</v>
       </c>
-      <c r="O50">
+      <c r="S50">
         <v>0.123457</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -3656,15 +3849,30 @@
         <v>16</v>
       </c>
       <c r="J51">
-        <f>SUM(G51, H51,I51)</f>
+        <f t="shared" si="2"/>
         <v>166</v>
       </c>
       <c r="K51">
-        <f>F51/J51</f>
+        <f t="shared" si="3"/>
         <v>0.8493975903614458</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L51" t="s">
+        <v>238</v>
+      </c>
+      <c r="P51">
+        <v>174</v>
+      </c>
+      <c r="Q51">
+        <v>0.224138</v>
+      </c>
+      <c r="R51">
+        <v>0.83950599999999997</v>
+      </c>
+      <c r="S51">
+        <v>0.123457</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -3693,15 +3901,18 @@
         <v>9</v>
       </c>
       <c r="J52">
-        <f>SUM(G52, H52,I52)</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="K52">
-        <f>F52/J52</f>
+        <f t="shared" si="3"/>
         <v>0.85263157894736841</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -3730,15 +3941,18 @@
         <v>7</v>
       </c>
       <c r="J53">
-        <f>SUM(G53, H53,I53)</f>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="K53">
-        <f>F53/J53</f>
+        <f t="shared" si="3"/>
         <v>0.84931506849315064</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L53" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -3767,20 +3981,22 @@
         <v>4</v>
       </c>
       <c r="J54">
-        <f>SUM(G54, H54,I54)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K54">
-        <f>F54/J54</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-      <c r="L54" s="4"/>
+      <c r="L54" s="4" t="s">
+        <v>238</v>
+      </c>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
       <c r="P54" s="4"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -3809,20 +4025,22 @@
         <v>4</v>
       </c>
       <c r="J55">
-        <f>SUM(G55, H55,I55)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K55">
-        <f>F55/J55</f>
+        <f t="shared" si="3"/>
         <v>0.84210526315789469</v>
       </c>
-      <c r="L55" s="5"/>
+      <c r="L55" s="5" t="s">
+        <v>238</v>
+      </c>
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
       <c r="P55" s="4"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -3851,20 +4069,22 @@
         <v>10</v>
       </c>
       <c r="J56">
-        <f>SUM(G56, H56,I56)</f>
+        <f t="shared" ref="J56:J87" si="4">SUM(G56, H56,I56)</f>
         <v>98</v>
       </c>
       <c r="K56">
-        <f>F56/J56</f>
+        <f t="shared" ref="K56:K87" si="5">F56/J56</f>
         <v>0.84693877551020413</v>
       </c>
-      <c r="L56" s="4"/>
+      <c r="L56" s="4" t="s">
+        <v>238</v>
+      </c>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
       <c r="P56" s="4"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -3893,20 +4113,22 @@
         <v>7</v>
       </c>
       <c r="J57">
-        <f>SUM(G57, H57,I57)</f>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="K57">
-        <f>F57/J57</f>
+        <f t="shared" si="5"/>
         <v>0.84931506849315064</v>
       </c>
-      <c r="L57" s="4"/>
+      <c r="L57" s="4" t="s">
+        <v>238</v>
+      </c>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -3935,15 +4157,18 @@
         <v>10</v>
       </c>
       <c r="J58">
-        <f>SUM(G58, H58,I58)</f>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="K58">
-        <f>F58/J58</f>
+        <f t="shared" si="5"/>
         <v>0.84375</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L58" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -3963,15 +4188,27 @@
         <v>145</v>
       </c>
       <c r="J59">
-        <f>SUM(G59, H59,I59)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K59" t="e">
-        <f>F59/J59</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L59" t="s">
+        <v>238</v>
+      </c>
+      <c r="N59">
+        <v>188</v>
+      </c>
+      <c r="O59">
+        <v>189</v>
+      </c>
+      <c r="P59">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>55</v>
       </c>
@@ -3991,15 +4228,30 @@
         <v>175</v>
       </c>
       <c r="J60">
-        <f>SUM(G60, H60,I60)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K60" t="e">
-        <f>F60/J60</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L60" t="s">
+        <v>238</v>
+      </c>
+      <c r="M60" t="s">
+        <v>239</v>
+      </c>
+      <c r="N60" t="s">
+        <v>238</v>
+      </c>
+      <c r="O60" t="s">
+        <v>238</v>
+      </c>
+      <c r="P60" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -4019,15 +4271,27 @@
         <v>174</v>
       </c>
       <c r="J61">
-        <f>SUM(G61, H61,I61)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K61" t="e">
-        <f>F61/J61</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L61" t="s">
+        <v>238</v>
+      </c>
+      <c r="M61" t="s">
+        <v>237</v>
+      </c>
+      <c r="N61" t="s">
+        <v>238</v>
+      </c>
+      <c r="O61" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -4047,15 +4311,18 @@
         <v>29</v>
       </c>
       <c r="J62">
-        <f>SUM(G62, H62,I62)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K62" t="e">
-        <f>F62/J62</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L62" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -4075,15 +4342,18 @@
         <v>29</v>
       </c>
       <c r="J63">
-        <f>SUM(G63, H63,I63)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K63" t="e">
-        <f>F63/J63</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L63" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -4103,15 +4373,18 @@
         <v>29</v>
       </c>
       <c r="J64">
-        <f>SUM(G64, H64,I64)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K64" t="e">
-        <f>F64/J64</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -4131,15 +4404,15 @@
         <v>58</v>
       </c>
       <c r="J65">
-        <f>SUM(G65, H65,I65)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K65" t="e">
-        <f>F65/J65</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>55</v>
       </c>
@@ -4159,15 +4432,15 @@
         <v>58</v>
       </c>
       <c r="J66">
-        <f>SUM(G66, H66,I66)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K66" t="e">
-        <f>F66/J66</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>55</v>
       </c>
@@ -4187,15 +4460,18 @@
         <v>116</v>
       </c>
       <c r="J67">
-        <f>SUM(G67, H67,I67)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K67" t="e">
-        <f>F67/J67</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -4215,15 +4491,18 @@
         <v>101</v>
       </c>
       <c r="J68">
-        <f>SUM(G68, H68,I68)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K68" t="e">
-        <f>F68/J68</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -4243,15 +4522,18 @@
         <v>77</v>
       </c>
       <c r="J69">
-        <f>SUM(G69, H69,I69)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K69" t="e">
-        <f>F69/J69</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -4271,15 +4553,18 @@
         <v>77</v>
       </c>
       <c r="J70">
-        <f>SUM(G70, H70,I70)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K70" t="e">
-        <f>F70/J70</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -4299,15 +4584,15 @@
         <v>50</v>
       </c>
       <c r="J71">
-        <f>SUM(G71, H71,I71)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K71" t="e">
-        <f>F71/J71</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -4327,15 +4612,15 @@
         <v>58</v>
       </c>
       <c r="J72">
-        <f>SUM(G72, H72,I72)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K72" t="e">
-        <f>F72/J72</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>55</v>
       </c>
@@ -4355,15 +4640,15 @@
         <v>42</v>
       </c>
       <c r="J73">
-        <f>SUM(G73, H73,I73)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K73" t="e">
-        <f>F73/J73</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>55</v>
       </c>
@@ -4383,15 +4668,30 @@
         <v>113</v>
       </c>
       <c r="J74">
-        <f>SUM(G74, H74,I74)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K74" t="e">
-        <f>F74/J74</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74" t="s">
+        <v>238</v>
+      </c>
+      <c r="N74">
+        <v>470</v>
+      </c>
+      <c r="O74">
+        <v>471</v>
+      </c>
+      <c r="P74">
+        <v>472</v>
+      </c>
+      <c r="Q74">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -4411,15 +4711,33 @@
         <v>88</v>
       </c>
       <c r="J75">
-        <f>SUM(G75, H75,I75)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K75" t="e">
-        <f>F75/J75</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75" t="s">
+        <v>238</v>
+      </c>
+      <c r="M75" t="s">
+        <v>239</v>
+      </c>
+      <c r="N75" t="s">
+        <v>238</v>
+      </c>
+      <c r="O75" t="s">
+        <v>238</v>
+      </c>
+      <c r="P75" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>55</v>
       </c>
@@ -4439,15 +4757,33 @@
         <v>119</v>
       </c>
       <c r="J76">
-        <f>SUM(G76, H76,I76)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K76" t="e">
-        <f>F76/J76</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76" t="s">
+        <v>238</v>
+      </c>
+      <c r="M76" t="s">
+        <v>237</v>
+      </c>
+      <c r="N76" t="s">
+        <v>238</v>
+      </c>
+      <c r="O76" t="s">
+        <v>238</v>
+      </c>
+      <c r="P76" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -4467,15 +4803,18 @@
         <v>20</v>
       </c>
       <c r="J77">
-        <f>SUM(G77, H77,I77)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K77" t="e">
-        <f>F77/J77</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>55</v>
       </c>
@@ -4495,15 +4834,18 @@
         <v>11</v>
       </c>
       <c r="J78">
-        <f>SUM(G78, H78,I78)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K78" t="e">
-        <f>F78/J78</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4523,15 +4865,18 @@
         <v>22</v>
       </c>
       <c r="J79">
-        <f>SUM(G79, H79,I79)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K79" t="e">
-        <f>F79/J79</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -4551,15 +4896,18 @@
         <v>22</v>
       </c>
       <c r="J80">
-        <f>SUM(G80, H80,I80)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K80" t="e">
-        <f>F80/J80</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -4579,15 +4927,18 @@
         <v>55</v>
       </c>
       <c r="J81">
-        <f>SUM(G81, H81,I81)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K81" t="e">
-        <f>F81/J81</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -4607,15 +4958,18 @@
         <v>20</v>
       </c>
       <c r="J82">
-        <f>SUM(G82, H82,I82)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K82" t="e">
-        <f>F82/J82</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -4635,15 +4989,18 @@
         <v>55</v>
       </c>
       <c r="J83">
-        <f>SUM(G83, H83,I83)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K83" t="e">
-        <f>F83/J83</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>55</v>
       </c>
@@ -4663,15 +5020,18 @@
         <v>20</v>
       </c>
       <c r="J84">
-        <f>SUM(G84, H84,I84)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K84" t="e">
-        <f>F84/J84</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>55</v>
       </c>
@@ -4691,15 +5051,18 @@
         <v>55</v>
       </c>
       <c r="J85">
-        <f>SUM(G85, H85,I85)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K85" t="e">
-        <f>F85/J85</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>55</v>
       </c>
@@ -4719,15 +5082,18 @@
         <v>23</v>
       </c>
       <c r="J86">
-        <f>SUM(G86, H86,I86)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K86" t="e">
-        <f>F86/J86</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>55</v>
       </c>
@@ -4747,15 +5113,18 @@
         <v>23</v>
       </c>
       <c r="J87">
-        <f>SUM(G87, H87,I87)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K87" t="e">
-        <f>F87/J87</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>55</v>
       </c>
@@ -4775,15 +5144,18 @@
         <v>22</v>
       </c>
       <c r="J88">
-        <f>SUM(G88, H88,I88)</f>
+        <f t="shared" ref="J88:J119" si="6">SUM(G88, H88,I88)</f>
         <v>0</v>
       </c>
       <c r="K88" t="e">
-        <f>F88/J88</f>
+        <f t="shared" ref="K88:K119" si="7">F88/J88</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>55</v>
       </c>
@@ -4803,15 +5175,18 @@
         <v>22</v>
       </c>
       <c r="J89">
-        <f>SUM(G89, H89,I89)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K89" t="e">
-        <f>F89/J89</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>55</v>
       </c>
@@ -4831,15 +5206,18 @@
         <v>22</v>
       </c>
       <c r="J90">
-        <f>SUM(G90, H90,I90)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K90" t="e">
-        <f>F90/J90</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>55</v>
       </c>
@@ -4859,15 +5237,18 @@
         <v>34</v>
       </c>
       <c r="J91">
-        <f>SUM(G91, H91,I91)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K91" t="e">
-        <f>F91/J91</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -4887,15 +5268,18 @@
         <v>54</v>
       </c>
       <c r="J92">
-        <f>SUM(G92, H92,I92)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K92" t="e">
-        <f>F92/J92</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L92" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>55</v>
       </c>
@@ -4915,15 +5299,30 @@
         <v>52</v>
       </c>
       <c r="J93">
-        <f>SUM(G93, H93,I93)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K93" t="e">
-        <f>F93/J93</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L93" t="s">
+        <v>238</v>
+      </c>
+      <c r="N93">
+        <v>212</v>
+      </c>
+      <c r="O93">
+        <v>213</v>
+      </c>
+      <c r="P93">
+        <v>214</v>
+      </c>
+      <c r="Q93">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>55</v>
       </c>
@@ -4943,15 +5342,33 @@
         <v>52</v>
       </c>
       <c r="J94">
-        <f>SUM(G94, H94,I94)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K94" t="e">
-        <f>F94/J94</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L94" t="s">
+        <v>238</v>
+      </c>
+      <c r="M94" t="s">
+        <v>239</v>
+      </c>
+      <c r="N94" t="s">
+        <v>238</v>
+      </c>
+      <c r="O94" t="s">
+        <v>238</v>
+      </c>
+      <c r="P94" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>55</v>
       </c>
@@ -4971,15 +5388,33 @@
         <v>24</v>
       </c>
       <c r="J95">
-        <f>SUM(G95, H95,I95)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K95" t="e">
-        <f>F95/J95</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L95" t="s">
+        <v>238</v>
+      </c>
+      <c r="M95" t="s">
+        <v>237</v>
+      </c>
+      <c r="N95" t="s">
+        <v>238</v>
+      </c>
+      <c r="O95" t="s">
+        <v>238</v>
+      </c>
+      <c r="P95" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>55</v>
       </c>
@@ -4999,15 +5434,33 @@
         <v>28</v>
       </c>
       <c r="J96">
-        <f>SUM(G96, H96,I96)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K96" t="e">
-        <f>F96/J96</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L96" t="s">
+        <v>238</v>
+      </c>
+      <c r="M96" t="s">
+        <v>240</v>
+      </c>
+      <c r="N96" t="s">
+        <v>238</v>
+      </c>
+      <c r="O96" t="s">
+        <v>238</v>
+      </c>
+      <c r="P96" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>55</v>
       </c>
@@ -5027,15 +5480,24 @@
         <v>28</v>
       </c>
       <c r="J97">
-        <f>SUM(G97, H97,I97)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K97" t="e">
-        <f>F97/J97</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L97" t="s">
+        <v>238</v>
+      </c>
+      <c r="M97" t="s">
+        <v>241</v>
+      </c>
+      <c r="N97" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>55</v>
       </c>
@@ -5055,15 +5517,18 @@
         <v>39</v>
       </c>
       <c r="J98">
-        <f>SUM(G98, H98,I98)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K98" t="e">
-        <f>F98/J98</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L98" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>55</v>
       </c>
@@ -5083,15 +5548,18 @@
         <v>24</v>
       </c>
       <c r="J99">
-        <f>SUM(G99, H99,I99)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K99" t="e">
-        <f>F99/J99</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L99" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>55</v>
       </c>
@@ -5111,15 +5579,18 @@
         <v>50</v>
       </c>
       <c r="J100">
-        <f>SUM(G100, H100,I100)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K100" t="e">
-        <f>F100/J100</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L100" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>55</v>
       </c>
@@ -5139,15 +5610,18 @@
         <v>74</v>
       </c>
       <c r="J101">
-        <f>SUM(G101, H101,I101)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K101" t="e">
-        <f>F101/J101</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L101" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>55</v>
       </c>
@@ -5167,15 +5641,18 @@
         <v>72</v>
       </c>
       <c r="J102">
-        <f>SUM(G102, H102,I102)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K102" t="e">
-        <f>F102/J102</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L102" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>55</v>
       </c>
@@ -5195,15 +5672,18 @@
         <v>35</v>
       </c>
       <c r="J103">
-        <f>SUM(G103, H103,I103)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K103" t="e">
-        <f>F103/J103</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L103" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>55</v>
       </c>
@@ -5223,15 +5703,18 @@
         <v>50</v>
       </c>
       <c r="J104">
-        <f>SUM(G104, H104,I104)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K104" t="e">
-        <f>F104/J104</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L104" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>55</v>
       </c>
@@ -5251,15 +5734,18 @@
         <v>50</v>
       </c>
       <c r="J105">
-        <f>SUM(G105, H105,I105)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K105" t="e">
-        <f>F105/J105</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L105" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>55</v>
       </c>
@@ -5279,15 +5765,18 @@
         <v>50</v>
       </c>
       <c r="J106">
-        <f>SUM(G106, H106,I106)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K106" t="e">
-        <f>F106/J106</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L106" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>55</v>
       </c>
@@ -5307,15 +5796,18 @@
         <v>40</v>
       </c>
       <c r="J107">
-        <f>SUM(G107, H107,I107)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K107" t="e">
-        <f>F107/J107</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L107" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>55</v>
       </c>
@@ -5335,15 +5827,18 @@
         <v>40</v>
       </c>
       <c r="J108">
-        <f>SUM(G108, H108,I108)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K108" t="e">
-        <f>F108/J108</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L108" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>55</v>
       </c>
@@ -5363,15 +5858,18 @@
         <v>40</v>
       </c>
       <c r="J109">
-        <f>SUM(G109, H109,I109)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K109" t="e">
-        <f>F109/J109</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L109" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>55</v>
       </c>
@@ -5391,15 +5889,18 @@
         <v>40</v>
       </c>
       <c r="J110">
-        <f>SUM(G110, H110,I110)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K110" t="e">
-        <f>F110/J110</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L110" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>55</v>
       </c>
@@ -5419,15 +5920,18 @@
         <v>67</v>
       </c>
       <c r="J111">
-        <f>SUM(G111, H111,I111)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K111" t="e">
-        <f>F111/J111</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L111" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>55</v>
       </c>
@@ -5447,15 +5951,18 @@
         <v>72</v>
       </c>
       <c r="J112">
-        <f>SUM(G112, H112,I112)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K112" t="e">
-        <f>F112/J112</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L112" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>55</v>
       </c>
@@ -5475,15 +5982,18 @@
         <v>26</v>
       </c>
       <c r="J113">
-        <f>SUM(G113, H113,I113)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K113" t="e">
-        <f>F113/J113</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L113" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>55</v>
       </c>
@@ -5503,15 +6013,18 @@
         <v>52</v>
       </c>
       <c r="J114">
-        <f>SUM(G114, H114,I114)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K114" t="e">
-        <f>F114/J114</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L114" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>55</v>
       </c>
@@ -5531,15 +6044,18 @@
         <v>48</v>
       </c>
       <c r="J115">
-        <f>SUM(G115, H115,I115)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K115" t="e">
-        <f>F115/J115</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L115" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>55</v>
       </c>
@@ -5559,15 +6075,18 @@
         <v>48</v>
       </c>
       <c r="J116">
-        <f>SUM(G116, H116,I116)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K116" t="e">
-        <f>F116/J116</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L116" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>55</v>
       </c>
@@ -5587,15 +6106,18 @@
         <v>50</v>
       </c>
       <c r="J117">
-        <f>SUM(G117, H117,I117)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K117" t="e">
-        <f>F117/J117</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L117" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>55</v>
       </c>
@@ -5615,15 +6137,18 @@
         <v>50</v>
       </c>
       <c r="J118">
-        <f>SUM(G118, H118,I118)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K118" t="e">
-        <f>F118/J118</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L118" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>55</v>
       </c>
@@ -5643,15 +6168,18 @@
         <v>50</v>
       </c>
       <c r="J119">
-        <f>SUM(G119, H119,I119)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K119" t="e">
-        <f>F119/J119</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L119" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>55</v>
       </c>
@@ -5671,15 +6199,18 @@
         <v>50</v>
       </c>
       <c r="J120">
-        <f>SUM(G120, H120,I120)</f>
+        <f t="shared" ref="J120:J151" si="8">SUM(G120, H120,I120)</f>
         <v>0</v>
       </c>
       <c r="K120" t="e">
-        <f>F120/J120</f>
+        <f t="shared" ref="K120:K151" si="9">F120/J120</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L120" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>55</v>
       </c>
@@ -5699,15 +6230,18 @@
         <v>26</v>
       </c>
       <c r="J121">
-        <f>SUM(G121, H121,I121)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K121" t="e">
-        <f>F121/J121</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L121" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>55</v>
       </c>
@@ -5727,15 +6261,18 @@
         <v>22</v>
       </c>
       <c r="J122">
-        <f>SUM(G122, H122,I122)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K122" t="e">
-        <f>F122/J122</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L122" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>55</v>
       </c>
@@ -5755,15 +6292,27 @@
         <v>34</v>
       </c>
       <c r="J123">
-        <f>SUM(G123, H123,I123)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K123" t="e">
-        <f>F123/J123</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L123" t="s">
+        <v>238</v>
+      </c>
+      <c r="N123">
+        <v>90</v>
+      </c>
+      <c r="O123">
+        <v>91</v>
+      </c>
+      <c r="P123">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>55</v>
       </c>
@@ -5783,15 +6332,30 @@
         <v>34</v>
       </c>
       <c r="J124">
-        <f>SUM(G124, H124,I124)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K124" t="e">
-        <f>F124/J124</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L124" t="s">
+        <v>238</v>
+      </c>
+      <c r="M124" t="s">
+        <v>239</v>
+      </c>
+      <c r="N124" t="s">
+        <v>238</v>
+      </c>
+      <c r="O124" t="s">
+        <v>238</v>
+      </c>
+      <c r="P124" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>55</v>
       </c>
@@ -5811,15 +6375,27 @@
         <v>34</v>
       </c>
       <c r="J125">
-        <f>SUM(G125, H125,I125)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K125" t="e">
-        <f>F125/J125</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L125" t="s">
+        <v>238</v>
+      </c>
+      <c r="M125" t="s">
+        <v>237</v>
+      </c>
+      <c r="N125" t="s">
+        <v>238</v>
+      </c>
+      <c r="O125" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>55</v>
       </c>
@@ -5839,15 +6415,18 @@
         <v>34</v>
       </c>
       <c r="J126">
-        <f>SUM(G126, H126,I126)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K126" t="e">
-        <f>F126/J126</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L126" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>55</v>
       </c>
@@ -5867,15 +6446,18 @@
         <v>30</v>
       </c>
       <c r="J127">
-        <f>SUM(G127, H127,I127)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K127" t="e">
-        <f>F127/J127</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L127" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>55</v>
       </c>
@@ -5895,15 +6477,15 @@
         <v>102</v>
       </c>
       <c r="J128">
-        <f>SUM(G128, H128,I128)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K128" t="e">
-        <f>F128/J128</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>55</v>
       </c>
@@ -5923,15 +6505,15 @@
         <v>34</v>
       </c>
       <c r="J129">
-        <f>SUM(G129, H129,I129)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K129" t="e">
-        <f>F129/J129</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>55</v>
       </c>
@@ -5951,15 +6533,18 @@
         <v>17</v>
       </c>
       <c r="J130">
-        <f>SUM(G130, H130,I130)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K130" t="e">
-        <f>F130/J130</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L130" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>55</v>
       </c>
@@ -5979,15 +6564,18 @@
         <v>17</v>
       </c>
       <c r="J131">
-        <f t="shared" ref="J131:J134" si="2">SUM(G131, H131,I131)</f>
+        <f t="shared" ref="J131:J134" si="10">SUM(G131, H131,I131)</f>
         <v>0</v>
       </c>
       <c r="K131" t="e">
-        <f t="shared" ref="K131:K134" si="3">F131/J131</f>
+        <f t="shared" ref="K131:K134" si="11">F131/J131</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L131" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>55</v>
       </c>
@@ -6007,15 +6595,18 @@
         <v>17</v>
       </c>
       <c r="J132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K132" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L132" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>55</v>
       </c>
@@ -6035,15 +6626,18 @@
         <v>15</v>
       </c>
       <c r="J133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K133" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L133" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>55</v>
       </c>
@@ -6063,15 +6657,18 @@
         <v>51</v>
       </c>
       <c r="J134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K134" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L134" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>55</v>
       </c>
@@ -6091,15 +6688,15 @@
         <v>66</v>
       </c>
       <c r="J135">
-        <f t="shared" ref="J135:J136" si="4">SUM(G135, H135,I135)</f>
+        <f t="shared" ref="J135:J136" si="12">SUM(G135, H135,I135)</f>
         <v>0</v>
       </c>
       <c r="K135" t="e">
-        <f t="shared" ref="K135:K136" si="5">F135/J135</f>
+        <f t="shared" ref="K135:K136" si="13">F135/J135</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>55</v>
       </c>
@@ -6119,15 +6716,15 @@
         <v>117</v>
       </c>
       <c r="J136">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K136" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>55</v>
       </c>
@@ -6154,8 +6751,11 @@
         <f>F137/J137</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L137" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>55</v>
       </c>
@@ -6175,15 +6775,18 @@
         <v>136</v>
       </c>
       <c r="J138">
-        <f t="shared" ref="J138:J141" si="6">SUM(G138, H138,I138)</f>
+        <f t="shared" ref="J138:J141" si="14">SUM(G138, H138,I138)</f>
         <v>0</v>
       </c>
       <c r="K138" t="e">
-        <f t="shared" ref="K138:K141" si="7">F138/J138</f>
+        <f t="shared" ref="K138:K141" si="15">F138/J138</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L138" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>55</v>
       </c>
@@ -6203,15 +6806,18 @@
         <v>150</v>
       </c>
       <c r="J139">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K139" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L139" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>55</v>
       </c>
@@ -6231,15 +6837,18 @@
         <v>133</v>
       </c>
       <c r="J140">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K140" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L140" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>55</v>
       </c>
@@ -6259,12 +6868,15 @@
         <v>99</v>
       </c>
       <c r="J141">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K141" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="L141" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -6279,8 +6891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add 4-wise comparison experiment
</commit_message>
<xml_diff>
--- a/document/Sales Launch.xlsx
+++ b/document/Sales Launch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" tabRatio="713" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" tabRatio="713" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Flat type" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="287">
   <si>
     <t>Quarterly</t>
   </si>
@@ -758,6 +758,138 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>423A</t>
+  </si>
+  <si>
+    <t>423B</t>
+  </si>
+  <si>
+    <t>653A</t>
+  </si>
+  <si>
+    <t>653B</t>
+  </si>
+  <si>
+    <t>653C</t>
+  </si>
+  <si>
+    <t>654C</t>
+  </si>
+  <si>
+    <t>654A</t>
+  </si>
+  <si>
+    <t>654B</t>
+  </si>
+  <si>
+    <t>654D</t>
+  </si>
+  <si>
+    <t>425A</t>
+  </si>
+  <si>
+    <t>425B</t>
+  </si>
+  <si>
+    <t>210B</t>
+  </si>
+  <si>
+    <t>211A</t>
+  </si>
+  <si>
+    <t>466A</t>
+  </si>
+  <si>
+    <t>209A</t>
+  </si>
+  <si>
+    <t>209B</t>
+  </si>
+  <si>
+    <t>210A</t>
+  </si>
+  <si>
+    <t>210C</t>
+  </si>
+  <si>
+    <t>465A</t>
+  </si>
+  <si>
+    <t>875B</t>
+  </si>
+  <si>
+    <t>876A</t>
+  </si>
+  <si>
+    <t>876C</t>
+  </si>
+  <si>
+    <t>874B</t>
+  </si>
+  <si>
+    <t>874C</t>
+  </si>
+  <si>
+    <t>874D</t>
+  </si>
+  <si>
+    <t>410A</t>
+  </si>
+  <si>
+    <t>411A</t>
+  </si>
+  <si>
+    <t>411B</t>
+  </si>
+  <si>
+    <t>655B</t>
+  </si>
+  <si>
+    <t>656A</t>
+  </si>
+  <si>
+    <t>656B</t>
+  </si>
+  <si>
+    <t>656C</t>
+  </si>
+  <si>
+    <t>657A</t>
+  </si>
+  <si>
+    <t>657B</t>
+  </si>
+  <si>
+    <t>655A</t>
+  </si>
+  <si>
+    <t>228A</t>
+  </si>
+  <si>
+    <t>228B</t>
+  </si>
+  <si>
+    <t>229A</t>
+  </si>
+  <si>
+    <t>229B</t>
+  </si>
+  <si>
+    <t>655C</t>
+  </si>
+  <si>
+    <t>Could not proceed further due to lack of information</t>
+  </si>
+  <si>
+    <t>Include 65 units of 3Gen flats</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>http://www.hdb.gov.sg/cs/infoweb/residential/buying-a-flat/new/application-status</t>
   </si>
 </sst>
 </file>
@@ -835,7 +967,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -843,6 +975,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -877,8 +1010,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table47" displayName="Table47" ref="A1:L142" totalsRowShown="0">
-  <autoFilter ref="A1:L142"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table47" displayName="Table47" ref="A1:L237" totalsRowShown="0">
+  <autoFilter ref="A1:L237"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Quarterly"/>
     <tableColumn id="2" name="Town"/>
@@ -902,8 +1035,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G45" totalsRowShown="0">
-  <autoFilter ref="A1:G45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G89" totalsRowShown="0">
+  <autoFilter ref="A1:G89"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Quarterly"/>
     <tableColumn id="2" name="Town"/>
@@ -1705,10 +1838,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T141"/>
+  <dimension ref="A1:T237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="M238" sqref="M238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1855,7 @@
     <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1760,7 +1893,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1800,7 +1933,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1837,7 +1970,7 @@
         <v>0.84210526315789469</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1873,14 +2006,8 @@
         <f t="shared" si="0"/>
         <v>0.84563758389261745</v>
       </c>
-      <c r="N4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1916,14 +2043,8 @@
         <f t="shared" si="0"/>
         <v>0.84393063583815031</v>
       </c>
-      <c r="N5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1959,17 +2080,8 @@
         <f t="shared" si="0"/>
         <v>0.85106382978723405</v>
       </c>
-      <c r="N6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2006,7 +2118,7 @@
         <v>0.84210526315789469</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2043,7 +2155,7 @@
         <v>0.85106382978723405</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2080,7 +2192,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2117,7 +2229,7 @@
         <v>0.84210526315789469</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2154,7 +2266,7 @@
         <v>0.82352941176470584</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2191,7 +2303,7 @@
         <v>0.81081081081081086</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2228,7 +2340,7 @@
         <v>0.84848484848484851</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2265,7 +2377,7 @@
         <v>0.85185185185185186</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2302,7 +2414,7 @@
         <v>0.84677419354838712</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2592,15 +2704,6 @@
       <c r="L23" t="s">
         <v>238</v>
       </c>
-      <c r="O23">
-        <v>170</v>
-      </c>
-      <c r="P23">
-        <v>171</v>
-      </c>
-      <c r="Q23">
-        <v>172</v>
-      </c>
       <c r="R23">
         <v>173</v>
       </c>
@@ -2650,18 +2753,6 @@
       <c r="L24" t="s">
         <v>238</v>
       </c>
-      <c r="N24" t="s">
-        <v>239</v>
-      </c>
-      <c r="O24" t="s">
-        <v>238</v>
-      </c>
-      <c r="P24" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>238</v>
-      </c>
       <c r="R24" t="s">
         <v>238</v>
       </c>
@@ -2711,18 +2802,6 @@
       <c r="L25" t="s">
         <v>238</v>
       </c>
-      <c r="N25" t="s">
-        <v>237</v>
-      </c>
-      <c r="O25" t="s">
-        <v>238</v>
-      </c>
-      <c r="P25" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>238</v>
-      </c>
       <c r="R25" t="s">
         <v>238</v>
       </c>
@@ -2772,12 +2851,6 @@
       <c r="L26" t="s">
         <v>238</v>
       </c>
-      <c r="N26" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>238</v>
-      </c>
       <c r="R26" t="s">
         <v>238</v>
       </c>
@@ -2819,12 +2892,6 @@
         <v>0.84210526315789469</v>
       </c>
       <c r="L27" t="s">
-        <v>238</v>
-      </c>
-      <c r="N27" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q27" t="s">
         <v>238</v>
       </c>
       <c r="R27" t="s">
@@ -4198,15 +4265,6 @@
       <c r="L59" t="s">
         <v>238</v>
       </c>
-      <c r="N59">
-        <v>188</v>
-      </c>
-      <c r="O59">
-        <v>189</v>
-      </c>
-      <c r="P59">
-        <v>187</v>
-      </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -4238,18 +4296,6 @@
       <c r="L60" t="s">
         <v>238</v>
       </c>
-      <c r="M60" t="s">
-        <v>239</v>
-      </c>
-      <c r="N60" t="s">
-        <v>238</v>
-      </c>
-      <c r="O60" t="s">
-        <v>238</v>
-      </c>
-      <c r="P60" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -4281,15 +4327,6 @@
       <c r="L61" t="s">
         <v>238</v>
       </c>
-      <c r="M61" t="s">
-        <v>237</v>
-      </c>
-      <c r="N61" t="s">
-        <v>238</v>
-      </c>
-      <c r="O61" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -4384,7 +4421,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -4412,7 +4449,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>55</v>
       </c>
@@ -4440,7 +4477,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>55</v>
       </c>
@@ -4471,7 +4508,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -4502,7 +4539,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -4533,7 +4570,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -4564,7 +4601,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -4592,7 +4629,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -4620,7 +4657,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>55</v>
       </c>
@@ -4648,7 +4685,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>55</v>
       </c>
@@ -4678,20 +4715,8 @@
       <c r="L74" t="s">
         <v>238</v>
       </c>
-      <c r="N74">
-        <v>470</v>
-      </c>
-      <c r="O74">
-        <v>471</v>
-      </c>
-      <c r="P74">
-        <v>472</v>
-      </c>
-      <c r="Q74">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -4721,23 +4746,8 @@
       <c r="L75" t="s">
         <v>238</v>
       </c>
-      <c r="M75" t="s">
-        <v>239</v>
-      </c>
-      <c r="N75" t="s">
-        <v>238</v>
-      </c>
-      <c r="O75" t="s">
-        <v>238</v>
-      </c>
-      <c r="P75" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>55</v>
       </c>
@@ -4767,23 +4777,8 @@
       <c r="L76" t="s">
         <v>238</v>
       </c>
-      <c r="M76" t="s">
-        <v>237</v>
-      </c>
-      <c r="N76" t="s">
-        <v>238</v>
-      </c>
-      <c r="O76" t="s">
-        <v>238</v>
-      </c>
-      <c r="P76" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -4814,7 +4809,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>55</v>
       </c>
@@ -4845,7 +4840,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4876,7 +4871,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -4907,7 +4902,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -4938,7 +4933,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -4969,7 +4964,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -5000,7 +4995,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>55</v>
       </c>
@@ -5031,7 +5026,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>55</v>
       </c>
@@ -5062,7 +5057,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>55</v>
       </c>
@@ -5093,7 +5088,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>55</v>
       </c>
@@ -5124,7 +5119,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>55</v>
       </c>
@@ -5155,7 +5150,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>55</v>
       </c>
@@ -5186,7 +5181,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>55</v>
       </c>
@@ -5217,7 +5212,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>55</v>
       </c>
@@ -5248,7 +5243,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -5279,7 +5274,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>55</v>
       </c>
@@ -5309,20 +5304,8 @@
       <c r="L93" t="s">
         <v>238</v>
       </c>
-      <c r="N93">
-        <v>212</v>
-      </c>
-      <c r="O93">
-        <v>213</v>
-      </c>
-      <c r="P93">
-        <v>214</v>
-      </c>
-      <c r="Q93">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>55</v>
       </c>
@@ -5352,23 +5335,8 @@
       <c r="L94" t="s">
         <v>238</v>
       </c>
-      <c r="M94" t="s">
-        <v>239</v>
-      </c>
-      <c r="N94" t="s">
-        <v>238</v>
-      </c>
-      <c r="O94" t="s">
-        <v>238</v>
-      </c>
-      <c r="P94" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>55</v>
       </c>
@@ -5398,23 +5366,8 @@
       <c r="L95" t="s">
         <v>238</v>
       </c>
-      <c r="M95" t="s">
-        <v>237</v>
-      </c>
-      <c r="N95" t="s">
-        <v>238</v>
-      </c>
-      <c r="O95" t="s">
-        <v>238</v>
-      </c>
-      <c r="P95" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>55</v>
       </c>
@@ -5444,23 +5397,8 @@
       <c r="L96" t="s">
         <v>238</v>
       </c>
-      <c r="M96" t="s">
-        <v>240</v>
-      </c>
-      <c r="N96" t="s">
-        <v>238</v>
-      </c>
-      <c r="O96" t="s">
-        <v>238</v>
-      </c>
-      <c r="P96" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>55</v>
       </c>
@@ -5490,14 +5428,8 @@
       <c r="L97" t="s">
         <v>238</v>
       </c>
-      <c r="M97" t="s">
-        <v>241</v>
-      </c>
-      <c r="N97" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>55</v>
       </c>
@@ -5528,7 +5460,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>55</v>
       </c>
@@ -5559,7 +5491,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>55</v>
       </c>
@@ -5590,7 +5522,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>55</v>
       </c>
@@ -5621,7 +5553,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>55</v>
       </c>
@@ -5652,7 +5584,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>55</v>
       </c>
@@ -5683,7 +5615,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>55</v>
       </c>
@@ -5714,7 +5646,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>55</v>
       </c>
@@ -5745,7 +5677,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>55</v>
       </c>
@@ -5776,7 +5708,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>55</v>
       </c>
@@ -5807,7 +5739,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>55</v>
       </c>
@@ -5838,7 +5770,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>55</v>
       </c>
@@ -5869,7 +5801,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>55</v>
       </c>
@@ -5900,7 +5832,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>55</v>
       </c>
@@ -5931,7 +5863,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>55</v>
       </c>
@@ -5962,7 +5894,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>55</v>
       </c>
@@ -5993,7 +5925,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>55</v>
       </c>
@@ -6024,7 +5956,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>55</v>
       </c>
@@ -6055,7 +5987,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>55</v>
       </c>
@@ -6086,7 +6018,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>55</v>
       </c>
@@ -6117,7 +6049,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>55</v>
       </c>
@@ -6148,7 +6080,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>55</v>
       </c>
@@ -6179,7 +6111,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>55</v>
       </c>
@@ -6199,18 +6131,18 @@
         <v>50</v>
       </c>
       <c r="J120">
-        <f t="shared" ref="J120:J151" si="8">SUM(G120, H120,I120)</f>
+        <f t="shared" ref="J120:J130" si="8">SUM(G120, H120,I120)</f>
         <v>0</v>
       </c>
       <c r="K120" t="e">
-        <f t="shared" ref="K120:K151" si="9">F120/J120</f>
+        <f t="shared" ref="K120:K130" si="9">F120/J120</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L120" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>55</v>
       </c>
@@ -6241,7 +6173,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>55</v>
       </c>
@@ -6272,7 +6204,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>55</v>
       </c>
@@ -6302,17 +6234,8 @@
       <c r="L123" t="s">
         <v>238</v>
       </c>
-      <c r="N123">
-        <v>90</v>
-      </c>
-      <c r="O123">
-        <v>91</v>
-      </c>
-      <c r="P123">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>55</v>
       </c>
@@ -6342,20 +6265,8 @@
       <c r="L124" t="s">
         <v>238</v>
       </c>
-      <c r="M124" t="s">
-        <v>239</v>
-      </c>
-      <c r="N124" t="s">
-        <v>238</v>
-      </c>
-      <c r="O124" t="s">
-        <v>238</v>
-      </c>
-      <c r="P124" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>55</v>
       </c>
@@ -6385,17 +6296,8 @@
       <c r="L125" t="s">
         <v>238</v>
       </c>
-      <c r="M125" t="s">
-        <v>237</v>
-      </c>
-      <c r="N125" t="s">
-        <v>238</v>
-      </c>
-      <c r="O125" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>55</v>
       </c>
@@ -6426,7 +6328,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>55</v>
       </c>
@@ -6457,7 +6359,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>55</v>
       </c>
@@ -6485,7 +6387,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>55</v>
       </c>
@@ -6513,7 +6415,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>55</v>
       </c>
@@ -6544,7 +6446,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>55</v>
       </c>
@@ -6575,7 +6477,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>55</v>
       </c>
@@ -6606,7 +6508,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>55</v>
       </c>
@@ -6637,7 +6539,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>55</v>
       </c>
@@ -6668,7 +6570,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>55</v>
       </c>
@@ -6696,7 +6598,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>55</v>
       </c>
@@ -6724,7 +6626,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>55</v>
       </c>
@@ -6755,7 +6657,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>55</v>
       </c>
@@ -6786,7 +6688,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>55</v>
       </c>
@@ -6817,7 +6719,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>55</v>
       </c>
@@ -6848,7 +6750,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>55</v>
       </c>
@@ -6877,6 +6779,2911 @@
       </c>
       <c r="L141" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>80</v>
+      </c>
+      <c r="B142" t="s">
+        <v>81</v>
+      </c>
+      <c r="C142" t="s">
+        <v>14</v>
+      </c>
+      <c r="D142" t="s">
+        <v>84</v>
+      </c>
+      <c r="E142" t="s">
+        <v>243</v>
+      </c>
+      <c r="F142">
+        <v>167</v>
+      </c>
+      <c r="L142" t="s">
+        <v>238</v>
+      </c>
+      <c r="N142">
+        <v>423</v>
+      </c>
+      <c r="O142">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>80</v>
+      </c>
+      <c r="B143" t="s">
+        <v>81</v>
+      </c>
+      <c r="C143" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" t="s">
+        <v>84</v>
+      </c>
+      <c r="E143" t="s">
+        <v>244</v>
+      </c>
+      <c r="F143">
+        <v>143</v>
+      </c>
+      <c r="J143">
+        <f>SUM(G143, H143,I143)</f>
+        <v>0</v>
+      </c>
+      <c r="K143" t="e">
+        <f>F143/J143</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L143" t="s">
+        <v>238</v>
+      </c>
+      <c r="M143" t="s">
+        <v>239</v>
+      </c>
+      <c r="N143" t="s">
+        <v>238</v>
+      </c>
+      <c r="O143" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>80</v>
+      </c>
+      <c r="B144" t="s">
+        <v>81</v>
+      </c>
+      <c r="C144" t="s">
+        <v>14</v>
+      </c>
+      <c r="D144" t="s">
+        <v>85</v>
+      </c>
+      <c r="E144" t="s">
+        <v>245</v>
+      </c>
+      <c r="F144">
+        <v>119</v>
+      </c>
+      <c r="J144">
+        <f>SUM(G144, H144,I144)</f>
+        <v>0</v>
+      </c>
+      <c r="K144" t="e">
+        <f>F144/J144</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L144" t="s">
+        <v>238</v>
+      </c>
+      <c r="N144" s="7">
+        <v>653</v>
+      </c>
+      <c r="O144">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>80</v>
+      </c>
+      <c r="B145" t="s">
+        <v>81</v>
+      </c>
+      <c r="C145" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" t="s">
+        <v>85</v>
+      </c>
+      <c r="E145" t="s">
+        <v>246</v>
+      </c>
+      <c r="F145">
+        <v>102</v>
+      </c>
+      <c r="J145">
+        <f>SUM(G145, H145,I145)</f>
+        <v>0</v>
+      </c>
+      <c r="K145" t="e">
+        <f>F145/J145</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L145" t="s">
+        <v>238</v>
+      </c>
+      <c r="M145" t="s">
+        <v>239</v>
+      </c>
+      <c r="N145" t="s">
+        <v>238</v>
+      </c>
+      <c r="O145" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>80</v>
+      </c>
+      <c r="B146" t="s">
+        <v>81</v>
+      </c>
+      <c r="C146" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" t="s">
+        <v>85</v>
+      </c>
+      <c r="E146" t="s">
+        <v>247</v>
+      </c>
+      <c r="F146">
+        <v>126</v>
+      </c>
+      <c r="J146">
+        <f>SUM(G146, H146,I146)</f>
+        <v>0</v>
+      </c>
+      <c r="K146" t="e">
+        <f>F146/J146</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L146" t="s">
+        <v>238</v>
+      </c>
+      <c r="M146" t="s">
+        <v>237</v>
+      </c>
+      <c r="N146" t="s">
+        <v>238</v>
+      </c>
+      <c r="O146" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>80</v>
+      </c>
+      <c r="B147" t="s">
+        <v>81</v>
+      </c>
+      <c r="C147" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147" t="s">
+        <v>85</v>
+      </c>
+      <c r="E147" t="s">
+        <v>248</v>
+      </c>
+      <c r="F147">
+        <v>56</v>
+      </c>
+      <c r="J147">
+        <f>SUM(G147, H147,I147)</f>
+        <v>0</v>
+      </c>
+      <c r="K147" t="e">
+        <f>F147/J147</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L147" t="s">
+        <v>238</v>
+      </c>
+      <c r="M147" t="s">
+        <v>240</v>
+      </c>
+      <c r="N147" t="s">
+        <v>238</v>
+      </c>
+      <c r="O147" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>80</v>
+      </c>
+      <c r="B148" t="s">
+        <v>81</v>
+      </c>
+      <c r="C148" t="s">
+        <v>6</v>
+      </c>
+      <c r="D148" t="s">
+        <v>84</v>
+      </c>
+      <c r="E148" t="s">
+        <v>243</v>
+      </c>
+      <c r="F148">
+        <v>24</v>
+      </c>
+      <c r="J148">
+        <f>SUM(G148, H148,I148)</f>
+        <v>0</v>
+      </c>
+      <c r="K148" t="e">
+        <f>F148/J148</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L148" t="s">
+        <v>238</v>
+      </c>
+      <c r="M148" t="s">
+        <v>237</v>
+      </c>
+      <c r="N148" t="s">
+        <v>238</v>
+      </c>
+      <c r="O148" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>80</v>
+      </c>
+      <c r="B149" t="s">
+        <v>81</v>
+      </c>
+      <c r="C149" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" t="s">
+        <v>84</v>
+      </c>
+      <c r="E149" t="s">
+        <v>244</v>
+      </c>
+      <c r="F149">
+        <v>48</v>
+      </c>
+      <c r="J149">
+        <f>SUM(G149, H149,I149)</f>
+        <v>0</v>
+      </c>
+      <c r="K149" t="e">
+        <f>F149/J149</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L149" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>80</v>
+      </c>
+      <c r="B150" t="s">
+        <v>81</v>
+      </c>
+      <c r="C150" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" t="s">
+        <v>84</v>
+      </c>
+      <c r="E150" t="s">
+        <v>252</v>
+      </c>
+      <c r="F150">
+        <v>21</v>
+      </c>
+      <c r="J150">
+        <f>SUM(G150, H150,I150)</f>
+        <v>0</v>
+      </c>
+      <c r="K150" t="e">
+        <f>F150/J150</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L150" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>80</v>
+      </c>
+      <c r="B151" t="s">
+        <v>81</v>
+      </c>
+      <c r="C151" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" t="s">
+        <v>84</v>
+      </c>
+      <c r="E151" t="s">
+        <v>253</v>
+      </c>
+      <c r="F151">
+        <v>21</v>
+      </c>
+      <c r="J151">
+        <f>SUM(G151, H151,I151)</f>
+        <v>0</v>
+      </c>
+      <c r="K151" t="e">
+        <f>F151/J151</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L151" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>80</v>
+      </c>
+      <c r="B152" t="s">
+        <v>81</v>
+      </c>
+      <c r="C152" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" t="s">
+        <v>85</v>
+      </c>
+      <c r="E152" t="s">
+        <v>246</v>
+      </c>
+      <c r="F152">
+        <v>34</v>
+      </c>
+      <c r="J152">
+        <f>SUM(G152, H152,I152)</f>
+        <v>0</v>
+      </c>
+      <c r="K152" t="e">
+        <f>F152/J152</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L152" t="s">
+        <v>238</v>
+      </c>
+      <c r="M152" t="s">
+        <v>241</v>
+      </c>
+      <c r="O152" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>80</v>
+      </c>
+      <c r="B153" t="s">
+        <v>81</v>
+      </c>
+      <c r="C153" t="s">
+        <v>6</v>
+      </c>
+      <c r="D153" t="s">
+        <v>85</v>
+      </c>
+      <c r="E153" t="s">
+        <v>249</v>
+      </c>
+      <c r="F153">
+        <v>14</v>
+      </c>
+      <c r="J153">
+        <f>SUM(G153, H153,I153)</f>
+        <v>0</v>
+      </c>
+      <c r="K153" t="e">
+        <f>F153/J153</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L153" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>80</v>
+      </c>
+      <c r="B154" t="s">
+        <v>81</v>
+      </c>
+      <c r="C154" t="s">
+        <v>6</v>
+      </c>
+      <c r="D154" t="s">
+        <v>85</v>
+      </c>
+      <c r="E154" t="s">
+        <v>250</v>
+      </c>
+      <c r="F154">
+        <v>10</v>
+      </c>
+      <c r="J154">
+        <f>SUM(G154, H154,I154)</f>
+        <v>0</v>
+      </c>
+      <c r="K154" t="e">
+        <f>F154/J154</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L154" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>80</v>
+      </c>
+      <c r="B155" t="s">
+        <v>81</v>
+      </c>
+      <c r="C155" t="s">
+        <v>6</v>
+      </c>
+      <c r="D155" t="s">
+        <v>85</v>
+      </c>
+      <c r="E155" t="s">
+        <v>248</v>
+      </c>
+      <c r="F155">
+        <v>21</v>
+      </c>
+      <c r="J155">
+        <f>SUM(G155, H155,I155)</f>
+        <v>0</v>
+      </c>
+      <c r="K155" t="e">
+        <f>F155/J155</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L155" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>80</v>
+      </c>
+      <c r="B156" t="s">
+        <v>81</v>
+      </c>
+      <c r="C156" t="s">
+        <v>6</v>
+      </c>
+      <c r="D156" t="s">
+        <v>85</v>
+      </c>
+      <c r="E156" t="s">
+        <v>251</v>
+      </c>
+      <c r="F156">
+        <v>16</v>
+      </c>
+      <c r="J156">
+        <f>SUM(G156, H156,I156)</f>
+        <v>0</v>
+      </c>
+      <c r="K156" t="e">
+        <f>F156/J156</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L156" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>80</v>
+      </c>
+      <c r="B157" t="s">
+        <v>81</v>
+      </c>
+      <c r="C157" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" t="s">
+        <v>84</v>
+      </c>
+      <c r="E157" t="s">
+        <v>243</v>
+      </c>
+      <c r="F157">
+        <v>49</v>
+      </c>
+      <c r="J157">
+        <f>SUM(G157, H157,I157)</f>
+        <v>0</v>
+      </c>
+      <c r="K157" t="e">
+        <f>F157/J157</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L157" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>80</v>
+      </c>
+      <c r="B158" t="s">
+        <v>81</v>
+      </c>
+      <c r="C158" t="s">
+        <v>7</v>
+      </c>
+      <c r="D158" t="s">
+        <v>84</v>
+      </c>
+      <c r="E158" t="s">
+        <v>252</v>
+      </c>
+      <c r="F158">
+        <v>64</v>
+      </c>
+      <c r="J158">
+        <f t="shared" ref="J158:J159" si="16">SUM(G158, H158,I158)</f>
+        <v>0</v>
+      </c>
+      <c r="K158" t="e">
+        <f t="shared" ref="K158:K159" si="17">F158/J158</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L158" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>80</v>
+      </c>
+      <c r="B159" t="s">
+        <v>81</v>
+      </c>
+      <c r="C159" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159" t="s">
+        <v>84</v>
+      </c>
+      <c r="E159" t="s">
+        <v>253</v>
+      </c>
+      <c r="F159">
+        <v>94</v>
+      </c>
+      <c r="J159">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="K159" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L159" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>80</v>
+      </c>
+      <c r="B160" t="s">
+        <v>81</v>
+      </c>
+      <c r="C160" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" t="s">
+        <v>85</v>
+      </c>
+      <c r="E160" t="s">
+        <v>245</v>
+      </c>
+      <c r="F160">
+        <v>70</v>
+      </c>
+      <c r="J160">
+        <f>SUM(G160, H160,I160)</f>
+        <v>0</v>
+      </c>
+      <c r="K160" t="e">
+        <f>F160/J160</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L160" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>80</v>
+      </c>
+      <c r="B161" t="s">
+        <v>81</v>
+      </c>
+      <c r="C161" t="s">
+        <v>7</v>
+      </c>
+      <c r="D161" t="s">
+        <v>85</v>
+      </c>
+      <c r="E161" t="s">
+        <v>246</v>
+      </c>
+      <c r="F161">
+        <v>70</v>
+      </c>
+      <c r="J161">
+        <f t="shared" ref="J161:J166" si="18">SUM(G161, H161,I161)</f>
+        <v>0</v>
+      </c>
+      <c r="K161" t="e">
+        <f t="shared" ref="K161:K166" si="19">F161/J161</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L161" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>80</v>
+      </c>
+      <c r="B162" t="s">
+        <v>81</v>
+      </c>
+      <c r="C162" t="s">
+        <v>7</v>
+      </c>
+      <c r="D162" t="s">
+        <v>85</v>
+      </c>
+      <c r="E162" t="s">
+        <v>247</v>
+      </c>
+      <c r="F162">
+        <v>68</v>
+      </c>
+      <c r="J162">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K162" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L162" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>80</v>
+      </c>
+      <c r="B163" t="s">
+        <v>81</v>
+      </c>
+      <c r="C163" t="s">
+        <v>7</v>
+      </c>
+      <c r="D163" t="s">
+        <v>85</v>
+      </c>
+      <c r="E163" t="s">
+        <v>249</v>
+      </c>
+      <c r="F163">
+        <v>98</v>
+      </c>
+      <c r="J163">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K163" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L163" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>80</v>
+      </c>
+      <c r="B164" t="s">
+        <v>81</v>
+      </c>
+      <c r="C164" t="s">
+        <v>7</v>
+      </c>
+      <c r="D164" t="s">
+        <v>85</v>
+      </c>
+      <c r="E164" t="s">
+        <v>250</v>
+      </c>
+      <c r="F164">
+        <v>86</v>
+      </c>
+      <c r="J164">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K164" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L164" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>80</v>
+      </c>
+      <c r="B165" t="s">
+        <v>81</v>
+      </c>
+      <c r="C165" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" t="s">
+        <v>85</v>
+      </c>
+      <c r="E165" t="s">
+        <v>248</v>
+      </c>
+      <c r="F165">
+        <v>28</v>
+      </c>
+      <c r="J165">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K165" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L165" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>80</v>
+      </c>
+      <c r="B166" t="s">
+        <v>81</v>
+      </c>
+      <c r="C166" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" t="s">
+        <v>85</v>
+      </c>
+      <c r="E166" t="s">
+        <v>251</v>
+      </c>
+      <c r="F166">
+        <v>96</v>
+      </c>
+      <c r="J166">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K166" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L166" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>80</v>
+      </c>
+      <c r="B167" t="s">
+        <v>82</v>
+      </c>
+      <c r="C167" t="s">
+        <v>6</v>
+      </c>
+      <c r="D167" t="s">
+        <v>87</v>
+      </c>
+      <c r="E167" t="s">
+        <v>254</v>
+      </c>
+      <c r="F167">
+        <v>50</v>
+      </c>
+      <c r="J167">
+        <f>SUM(G167, H167,I167)</f>
+        <v>0</v>
+      </c>
+      <c r="K167" t="e">
+        <f>F167/J167</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L167" t="s">
+        <v>238</v>
+      </c>
+      <c r="N167">
+        <v>209</v>
+      </c>
+      <c r="O167">
+        <v>210</v>
+      </c>
+      <c r="P167">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>80</v>
+      </c>
+      <c r="B168" t="s">
+        <v>82</v>
+      </c>
+      <c r="C168" t="s">
+        <v>6</v>
+      </c>
+      <c r="D168" t="s">
+        <v>87</v>
+      </c>
+      <c r="E168" t="s">
+        <v>255</v>
+      </c>
+      <c r="F168">
+        <v>98</v>
+      </c>
+      <c r="J168">
+        <f>SUM(G168, H168,I168)</f>
+        <v>0</v>
+      </c>
+      <c r="K168" t="e">
+        <f>F168/J168</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L168" t="s">
+        <v>238</v>
+      </c>
+      <c r="M168" t="s">
+        <v>239</v>
+      </c>
+      <c r="N168" t="s">
+        <v>238</v>
+      </c>
+      <c r="O168" t="s">
+        <v>238</v>
+      </c>
+      <c r="P168" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>80</v>
+      </c>
+      <c r="B169" t="s">
+        <v>82</v>
+      </c>
+      <c r="C169" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169" t="s">
+        <v>88</v>
+      </c>
+      <c r="E169" t="s">
+        <v>256</v>
+      </c>
+      <c r="F169">
+        <v>70</v>
+      </c>
+      <c r="J169">
+        <f>SUM(G169, H169,I169)</f>
+        <v>0</v>
+      </c>
+      <c r="K169" t="e">
+        <f>F169/J169</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>80</v>
+      </c>
+      <c r="B170" t="s">
+        <v>82</v>
+      </c>
+      <c r="C170" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" t="s">
+        <v>87</v>
+      </c>
+      <c r="E170" t="s">
+        <v>257</v>
+      </c>
+      <c r="F170">
+        <v>76</v>
+      </c>
+      <c r="J170">
+        <f>SUM(G170, H170,I170)</f>
+        <v>0</v>
+      </c>
+      <c r="K170" t="e">
+        <f>F170/J170</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L170" t="s">
+        <v>238</v>
+      </c>
+      <c r="M170" t="s">
+        <v>237</v>
+      </c>
+      <c r="N170" t="s">
+        <v>238</v>
+      </c>
+      <c r="O170" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>80</v>
+      </c>
+      <c r="B171" t="s">
+        <v>82</v>
+      </c>
+      <c r="C171" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" t="s">
+        <v>87</v>
+      </c>
+      <c r="E171" t="s">
+        <v>258</v>
+      </c>
+      <c r="F171">
+        <v>76</v>
+      </c>
+      <c r="J171">
+        <f>SUM(G171, H171,I171)</f>
+        <v>0</v>
+      </c>
+      <c r="K171" t="e">
+        <f>F171/J171</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L171" t="s">
+        <v>238</v>
+      </c>
+      <c r="M171" t="s">
+        <v>240</v>
+      </c>
+      <c r="O171" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>80</v>
+      </c>
+      <c r="B172" t="s">
+        <v>82</v>
+      </c>
+      <c r="C172" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" t="s">
+        <v>87</v>
+      </c>
+      <c r="E172" t="s">
+        <v>259</v>
+      </c>
+      <c r="F172">
+        <v>131</v>
+      </c>
+      <c r="J172">
+        <f>SUM(G172, H172,I172)</f>
+        <v>0</v>
+      </c>
+      <c r="K172" t="e">
+        <f>F172/J172</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L172" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>80</v>
+      </c>
+      <c r="B173" t="s">
+        <v>82</v>
+      </c>
+      <c r="C173" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" t="s">
+        <v>87</v>
+      </c>
+      <c r="E173" t="s">
+        <v>254</v>
+      </c>
+      <c r="F173">
+        <v>168</v>
+      </c>
+      <c r="J173">
+        <f>SUM(G173, H173,I173)</f>
+        <v>0</v>
+      </c>
+      <c r="K173" t="e">
+        <f>F173/J173</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L173" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>80</v>
+      </c>
+      <c r="B174" t="s">
+        <v>82</v>
+      </c>
+      <c r="C174" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" t="s">
+        <v>87</v>
+      </c>
+      <c r="E174" t="s">
+        <v>260</v>
+      </c>
+      <c r="F174">
+        <v>38</v>
+      </c>
+      <c r="J174">
+        <f>SUM(G174, H174,I174)</f>
+        <v>0</v>
+      </c>
+      <c r="K174" t="e">
+        <f>F174/J174</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L174" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>80</v>
+      </c>
+      <c r="B175" t="s">
+        <v>82</v>
+      </c>
+      <c r="C175" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" t="s">
+        <v>87</v>
+      </c>
+      <c r="E175" t="s">
+        <v>255</v>
+      </c>
+      <c r="F175">
+        <v>40</v>
+      </c>
+      <c r="J175">
+        <f>SUM(G175, H175,I175)</f>
+        <v>0</v>
+      </c>
+      <c r="K175" t="e">
+        <f>F175/J175</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L175" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>80</v>
+      </c>
+      <c r="B176" t="s">
+        <v>82</v>
+      </c>
+      <c r="C176" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" t="s">
+        <v>88</v>
+      </c>
+      <c r="E176" t="s">
+        <v>261</v>
+      </c>
+      <c r="F176">
+        <v>195</v>
+      </c>
+      <c r="J176">
+        <f>SUM(G176, H176,I176)</f>
+        <v>0</v>
+      </c>
+      <c r="K176" t="e">
+        <f>F176/J176</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>80</v>
+      </c>
+      <c r="B177" t="s">
+        <v>82</v>
+      </c>
+      <c r="C177" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" t="s">
+        <v>88</v>
+      </c>
+      <c r="E177" t="s">
+        <v>256</v>
+      </c>
+      <c r="F177">
+        <v>42</v>
+      </c>
+      <c r="J177">
+        <f>SUM(G177, H177,I177)</f>
+        <v>0</v>
+      </c>
+      <c r="K177" t="e">
+        <f>F177/J177</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>80</v>
+      </c>
+      <c r="B178" t="s">
+        <v>82</v>
+      </c>
+      <c r="C178" t="s">
+        <v>8</v>
+      </c>
+      <c r="D178" t="s">
+        <v>87</v>
+      </c>
+      <c r="E178" t="s">
+        <v>257</v>
+      </c>
+      <c r="F178">
+        <v>76</v>
+      </c>
+      <c r="J178">
+        <f>SUM(G178, H178,I178)</f>
+        <v>0</v>
+      </c>
+      <c r="K178" t="e">
+        <f>F178/J178</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L178" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>80</v>
+      </c>
+      <c r="B179" t="s">
+        <v>82</v>
+      </c>
+      <c r="C179" t="s">
+        <v>8</v>
+      </c>
+      <c r="D179" t="s">
+        <v>87</v>
+      </c>
+      <c r="E179" t="s">
+        <v>258</v>
+      </c>
+      <c r="F179">
+        <v>76</v>
+      </c>
+      <c r="J179">
+        <f>SUM(G179, H179,I179)</f>
+        <v>0</v>
+      </c>
+      <c r="K179" t="e">
+        <f>F179/J179</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L179" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>80</v>
+      </c>
+      <c r="B180" t="s">
+        <v>82</v>
+      </c>
+      <c r="C180" t="s">
+        <v>8</v>
+      </c>
+      <c r="D180" t="s">
+        <v>87</v>
+      </c>
+      <c r="E180" t="s">
+        <v>259</v>
+      </c>
+      <c r="F180">
+        <v>124</v>
+      </c>
+      <c r="J180">
+        <f>SUM(G180, H180,I180)</f>
+        <v>0</v>
+      </c>
+      <c r="K180" t="e">
+        <f>F180/J180</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L180" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>80</v>
+      </c>
+      <c r="B181" t="s">
+        <v>82</v>
+      </c>
+      <c r="C181" t="s">
+        <v>8</v>
+      </c>
+      <c r="D181" t="s">
+        <v>87</v>
+      </c>
+      <c r="E181" t="s">
+        <v>254</v>
+      </c>
+      <c r="F181">
+        <v>62</v>
+      </c>
+      <c r="J181">
+        <f>SUM(G181, H181,I181)</f>
+        <v>0</v>
+      </c>
+      <c r="K181" t="e">
+        <f>F181/J181</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L181" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>80</v>
+      </c>
+      <c r="B182" t="s">
+        <v>82</v>
+      </c>
+      <c r="C182" t="s">
+        <v>8</v>
+      </c>
+      <c r="D182" t="s">
+        <v>87</v>
+      </c>
+      <c r="E182" t="s">
+        <v>260</v>
+      </c>
+      <c r="F182">
+        <v>115</v>
+      </c>
+      <c r="J182">
+        <f>SUM(G182, H182,I182)</f>
+        <v>0</v>
+      </c>
+      <c r="K182" t="e">
+        <f>F182/J182</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L182" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>80</v>
+      </c>
+      <c r="B183" t="s">
+        <v>82</v>
+      </c>
+      <c r="C183" t="s">
+        <v>8</v>
+      </c>
+      <c r="D183" t="s">
+        <v>87</v>
+      </c>
+      <c r="E183" t="s">
+        <v>255</v>
+      </c>
+      <c r="F183">
+        <v>49</v>
+      </c>
+      <c r="J183">
+        <f>SUM(G183, H183,I183)</f>
+        <v>0</v>
+      </c>
+      <c r="K183" t="e">
+        <f>F183/J183</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L183" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>80</v>
+      </c>
+      <c r="B184" t="s">
+        <v>82</v>
+      </c>
+      <c r="C184" t="s">
+        <v>8</v>
+      </c>
+      <c r="D184" t="s">
+        <v>88</v>
+      </c>
+      <c r="E184" t="s">
+        <v>261</v>
+      </c>
+      <c r="F184">
+        <v>117</v>
+      </c>
+      <c r="J184">
+        <f>SUM(G184, H184,I184)</f>
+        <v>0</v>
+      </c>
+      <c r="K184" t="e">
+        <f>F184/J184</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>80</v>
+      </c>
+      <c r="B185" t="s">
+        <v>83</v>
+      </c>
+      <c r="C185" t="s">
+        <v>7</v>
+      </c>
+      <c r="D185" t="s">
+        <v>91</v>
+      </c>
+      <c r="E185" t="s">
+        <v>262</v>
+      </c>
+      <c r="F185">
+        <v>41</v>
+      </c>
+      <c r="J185">
+        <f>SUM(G185, H185,I185)</f>
+        <v>0</v>
+      </c>
+      <c r="K185" t="e">
+        <f>F185/J185</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L185" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>80</v>
+      </c>
+      <c r="B186" t="s">
+        <v>83</v>
+      </c>
+      <c r="C186" t="s">
+        <v>7</v>
+      </c>
+      <c r="D186" t="s">
+        <v>91</v>
+      </c>
+      <c r="E186" t="s">
+        <v>263</v>
+      </c>
+      <c r="F186">
+        <v>56</v>
+      </c>
+      <c r="J186">
+        <f>SUM(G186, H186,I186)</f>
+        <v>0</v>
+      </c>
+      <c r="K186" t="e">
+        <f>F186/J186</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L186" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>80</v>
+      </c>
+      <c r="B187" t="s">
+        <v>83</v>
+      </c>
+      <c r="C187" t="s">
+        <v>7</v>
+      </c>
+      <c r="D187" t="s">
+        <v>91</v>
+      </c>
+      <c r="E187" t="s">
+        <v>264</v>
+      </c>
+      <c r="F187">
+        <v>56</v>
+      </c>
+      <c r="J187">
+        <f>SUM(G187, H187,I187)</f>
+        <v>0</v>
+      </c>
+      <c r="K187" t="e">
+        <f>F187/J187</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L187" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>80</v>
+      </c>
+      <c r="B188" t="s">
+        <v>83</v>
+      </c>
+      <c r="C188" t="s">
+        <v>7</v>
+      </c>
+      <c r="D188" t="s">
+        <v>92</v>
+      </c>
+      <c r="E188" t="s">
+        <v>265</v>
+      </c>
+      <c r="F188">
+        <v>41</v>
+      </c>
+      <c r="J188">
+        <f>SUM(G188, H188,I188)</f>
+        <v>0</v>
+      </c>
+      <c r="K188" t="e">
+        <f>F188/J188</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L188" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>80</v>
+      </c>
+      <c r="B189" t="s">
+        <v>83</v>
+      </c>
+      <c r="C189" t="s">
+        <v>7</v>
+      </c>
+      <c r="D189" t="s">
+        <v>92</v>
+      </c>
+      <c r="E189" t="s">
+        <v>266</v>
+      </c>
+      <c r="F189">
+        <v>56</v>
+      </c>
+      <c r="J189">
+        <f>SUM(G189, H189,I189)</f>
+        <v>0</v>
+      </c>
+      <c r="K189" t="e">
+        <f>F189/J189</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L189" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>80</v>
+      </c>
+      <c r="B190" t="s">
+        <v>83</v>
+      </c>
+      <c r="C190" t="s">
+        <v>7</v>
+      </c>
+      <c r="D190" t="s">
+        <v>92</v>
+      </c>
+      <c r="E190" t="s">
+        <v>267</v>
+      </c>
+      <c r="F190">
+        <v>56</v>
+      </c>
+      <c r="J190">
+        <f>SUM(G190, H190,I190)</f>
+        <v>0</v>
+      </c>
+      <c r="K190" t="e">
+        <f>F190/J190</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L190" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>80</v>
+      </c>
+      <c r="B191" t="s">
+        <v>83</v>
+      </c>
+      <c r="C191" t="s">
+        <v>8</v>
+      </c>
+      <c r="D191" t="s">
+        <v>91</v>
+      </c>
+      <c r="E191" t="s">
+        <v>262</v>
+      </c>
+      <c r="F191">
+        <v>55</v>
+      </c>
+      <c r="J191">
+        <f>SUM(G191, H191,I191)</f>
+        <v>0</v>
+      </c>
+      <c r="K191" t="e">
+        <f>F191/J191</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L191" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>80</v>
+      </c>
+      <c r="B192" t="s">
+        <v>83</v>
+      </c>
+      <c r="C192" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" t="s">
+        <v>91</v>
+      </c>
+      <c r="E192" t="s">
+        <v>263</v>
+      </c>
+      <c r="F192">
+        <v>56</v>
+      </c>
+      <c r="J192">
+        <f>SUM(G192, H192,I192)</f>
+        <v>0</v>
+      </c>
+      <c r="K192" t="e">
+        <f>F192/J192</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L192" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>80</v>
+      </c>
+      <c r="B193" t="s">
+        <v>83</v>
+      </c>
+      <c r="C193" t="s">
+        <v>8</v>
+      </c>
+      <c r="D193" t="s">
+        <v>91</v>
+      </c>
+      <c r="E193" t="s">
+        <v>264</v>
+      </c>
+      <c r="F193">
+        <v>55</v>
+      </c>
+      <c r="J193">
+        <f>SUM(G193, H193,I193)</f>
+        <v>0</v>
+      </c>
+      <c r="K193" t="e">
+        <f>F193/J193</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L193" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>80</v>
+      </c>
+      <c r="B194" t="s">
+        <v>83</v>
+      </c>
+      <c r="C194" t="s">
+        <v>8</v>
+      </c>
+      <c r="D194" t="s">
+        <v>92</v>
+      </c>
+      <c r="E194" t="s">
+        <v>265</v>
+      </c>
+      <c r="F194">
+        <v>55</v>
+      </c>
+      <c r="J194">
+        <f>SUM(G194, H194,I194)</f>
+        <v>0</v>
+      </c>
+      <c r="K194" t="e">
+        <f>F194/J194</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L194" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>80</v>
+      </c>
+      <c r="B195" t="s">
+        <v>83</v>
+      </c>
+      <c r="C195" t="s">
+        <v>8</v>
+      </c>
+      <c r="D195" t="s">
+        <v>92</v>
+      </c>
+      <c r="E195" t="s">
+        <v>266</v>
+      </c>
+      <c r="F195">
+        <v>56</v>
+      </c>
+      <c r="J195">
+        <f>SUM(G195, H195,I195)</f>
+        <v>0</v>
+      </c>
+      <c r="K195" t="e">
+        <f>F195/J195</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L195" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>80</v>
+      </c>
+      <c r="B196" t="s">
+        <v>83</v>
+      </c>
+      <c r="C196" t="s">
+        <v>8</v>
+      </c>
+      <c r="D196" t="s">
+        <v>92</v>
+      </c>
+      <c r="E196" t="s">
+        <v>267</v>
+      </c>
+      <c r="F196">
+        <v>55</v>
+      </c>
+      <c r="J196">
+        <f>SUM(G196, H196,I196)</f>
+        <v>0</v>
+      </c>
+      <c r="K196" t="e">
+        <f>F196/J196</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L196" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>94</v>
+      </c>
+      <c r="B197" t="s">
+        <v>81</v>
+      </c>
+      <c r="C197" t="s">
+        <v>14</v>
+      </c>
+      <c r="D197" t="s">
+        <v>98</v>
+      </c>
+      <c r="E197" t="s">
+        <v>268</v>
+      </c>
+      <c r="F197">
+        <v>64</v>
+      </c>
+      <c r="J197">
+        <f>SUM(G197, H197,I197)</f>
+        <v>0</v>
+      </c>
+      <c r="K197" t="e">
+        <f>F197/J197</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>94</v>
+      </c>
+      <c r="B198" t="s">
+        <v>81</v>
+      </c>
+      <c r="C198" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" t="s">
+        <v>98</v>
+      </c>
+      <c r="E198" t="s">
+        <v>269</v>
+      </c>
+      <c r="F198">
+        <v>65</v>
+      </c>
+      <c r="J198">
+        <f>SUM(G198, H198,I198)</f>
+        <v>0</v>
+      </c>
+      <c r="K198" t="e">
+        <f>F198/J198</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>94</v>
+      </c>
+      <c r="B199" t="s">
+        <v>81</v>
+      </c>
+      <c r="C199" t="s">
+        <v>14</v>
+      </c>
+      <c r="D199" t="s">
+        <v>98</v>
+      </c>
+      <c r="E199" t="s">
+        <v>270</v>
+      </c>
+      <c r="F199">
+        <v>66</v>
+      </c>
+      <c r="J199">
+        <f>SUM(G199, H199,I199)</f>
+        <v>0</v>
+      </c>
+      <c r="K199" t="e">
+        <f>F199/J199</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>94</v>
+      </c>
+      <c r="B200" t="s">
+        <v>81</v>
+      </c>
+      <c r="C200" t="s">
+        <v>14</v>
+      </c>
+      <c r="D200" t="s">
+        <v>99</v>
+      </c>
+      <c r="E200" t="s">
+        <v>271</v>
+      </c>
+      <c r="F200">
+        <v>118</v>
+      </c>
+      <c r="J200">
+        <f>SUM(G200, H200,I200)</f>
+        <v>0</v>
+      </c>
+      <c r="K200" t="e">
+        <f>F200/J200</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>94</v>
+      </c>
+      <c r="B201" t="s">
+        <v>81</v>
+      </c>
+      <c r="C201" t="s">
+        <v>14</v>
+      </c>
+      <c r="D201" t="s">
+        <v>99</v>
+      </c>
+      <c r="E201" t="s">
+        <v>272</v>
+      </c>
+      <c r="F201">
+        <v>119</v>
+      </c>
+      <c r="J201">
+        <f>SUM(G201, H201,I201)</f>
+        <v>0</v>
+      </c>
+      <c r="K201" t="e">
+        <f>F201/J201</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>94</v>
+      </c>
+      <c r="B202" t="s">
+        <v>81</v>
+      </c>
+      <c r="C202" t="s">
+        <v>14</v>
+      </c>
+      <c r="D202" t="s">
+        <v>99</v>
+      </c>
+      <c r="E202" t="s">
+        <v>273</v>
+      </c>
+      <c r="F202">
+        <v>102</v>
+      </c>
+      <c r="J202">
+        <f>SUM(G202, H202,I202)</f>
+        <v>0</v>
+      </c>
+      <c r="K202" t="e">
+        <f>F202/J202</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>94</v>
+      </c>
+      <c r="B203" t="s">
+        <v>81</v>
+      </c>
+      <c r="C203" t="s">
+        <v>14</v>
+      </c>
+      <c r="D203" t="s">
+        <v>99</v>
+      </c>
+      <c r="E203" t="s">
+        <v>274</v>
+      </c>
+      <c r="F203">
+        <v>122</v>
+      </c>
+      <c r="J203">
+        <f>SUM(G203, H203,I203)</f>
+        <v>0</v>
+      </c>
+      <c r="K203" t="e">
+        <f>F203/J203</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>94</v>
+      </c>
+      <c r="B204" t="s">
+        <v>81</v>
+      </c>
+      <c r="C204" t="s">
+        <v>14</v>
+      </c>
+      <c r="D204" t="s">
+        <v>99</v>
+      </c>
+      <c r="E204" t="s">
+        <v>275</v>
+      </c>
+      <c r="F204">
+        <v>90</v>
+      </c>
+      <c r="J204">
+        <f>SUM(G204, H204,I204)</f>
+        <v>0</v>
+      </c>
+      <c r="K204" t="e">
+        <f>F204/J204</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>94</v>
+      </c>
+      <c r="B205" t="s">
+        <v>81</v>
+      </c>
+      <c r="C205" t="s">
+        <v>14</v>
+      </c>
+      <c r="D205" t="s">
+        <v>99</v>
+      </c>
+      <c r="E205" t="s">
+        <v>276</v>
+      </c>
+      <c r="F205">
+        <v>118</v>
+      </c>
+      <c r="J205">
+        <f>SUM(G205, H205,I205)</f>
+        <v>0</v>
+      </c>
+      <c r="K205" t="e">
+        <f>F205/J205</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>94</v>
+      </c>
+      <c r="B206" t="s">
+        <v>81</v>
+      </c>
+      <c r="C206" t="s">
+        <v>6</v>
+      </c>
+      <c r="D206" t="s">
+        <v>98</v>
+      </c>
+      <c r="E206" t="s">
+        <v>268</v>
+      </c>
+      <c r="F206">
+        <v>47</v>
+      </c>
+      <c r="J206">
+        <f>SUM(G206, H206,I206)</f>
+        <v>0</v>
+      </c>
+      <c r="K206" t="e">
+        <f>F206/J206</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>94</v>
+      </c>
+      <c r="B207" t="s">
+        <v>81</v>
+      </c>
+      <c r="C207" t="s">
+        <v>6</v>
+      </c>
+      <c r="D207" t="s">
+        <v>98</v>
+      </c>
+      <c r="E207" t="s">
+        <v>269</v>
+      </c>
+      <c r="F207">
+        <v>23</v>
+      </c>
+      <c r="J207">
+        <f>SUM(G207, H207,I207)</f>
+        <v>0</v>
+      </c>
+      <c r="K207" t="e">
+        <f>F207/J207</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>94</v>
+      </c>
+      <c r="B208" t="s">
+        <v>81</v>
+      </c>
+      <c r="C208" t="s">
+        <v>6</v>
+      </c>
+      <c r="D208" t="s">
+        <v>98</v>
+      </c>
+      <c r="E208" t="s">
+        <v>270</v>
+      </c>
+      <c r="F208">
+        <v>23</v>
+      </c>
+      <c r="J208">
+        <f>SUM(G208, H208,I208)</f>
+        <v>0</v>
+      </c>
+      <c r="K208" t="e">
+        <f>F208/J208</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>94</v>
+      </c>
+      <c r="B209" t="s">
+        <v>81</v>
+      </c>
+      <c r="C209" t="s">
+        <v>6</v>
+      </c>
+      <c r="D209" t="s">
+        <v>99</v>
+      </c>
+      <c r="E209" t="s">
+        <v>277</v>
+      </c>
+      <c r="F209">
+        <v>16</v>
+      </c>
+      <c r="J209">
+        <f>SUM(G209, H209,I209)</f>
+        <v>0</v>
+      </c>
+      <c r="K209" t="e">
+        <f>F209/J209</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>94</v>
+      </c>
+      <c r="B210" t="s">
+        <v>81</v>
+      </c>
+      <c r="C210" t="s">
+        <v>6</v>
+      </c>
+      <c r="D210" t="s">
+        <v>99</v>
+      </c>
+      <c r="E210" t="s">
+        <v>273</v>
+      </c>
+      <c r="F210">
+        <v>34</v>
+      </c>
+      <c r="J210">
+        <f>SUM(G210, H210,I210)</f>
+        <v>0</v>
+      </c>
+      <c r="K210" t="e">
+        <f>F210/J210</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>94</v>
+      </c>
+      <c r="B211" t="s">
+        <v>81</v>
+      </c>
+      <c r="C211" t="s">
+        <v>6</v>
+      </c>
+      <c r="D211" t="s">
+        <v>99</v>
+      </c>
+      <c r="E211" t="s">
+        <v>275</v>
+      </c>
+      <c r="F211">
+        <v>30</v>
+      </c>
+      <c r="J211">
+        <f>SUM(G211, H211,I211)</f>
+        <v>0</v>
+      </c>
+      <c r="K211" t="e">
+        <f>F211/J211</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>94</v>
+      </c>
+      <c r="B212" t="s">
+        <v>81</v>
+      </c>
+      <c r="C212" t="s">
+        <v>7</v>
+      </c>
+      <c r="D212" t="s">
+        <v>97</v>
+      </c>
+      <c r="E212" t="s">
+        <v>278</v>
+      </c>
+      <c r="F212">
+        <v>48</v>
+      </c>
+      <c r="J212">
+        <f>SUM(G212, H212,I212)</f>
+        <v>0</v>
+      </c>
+      <c r="K212" t="e">
+        <f>F212/J212</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>94</v>
+      </c>
+      <c r="B213" t="s">
+        <v>81</v>
+      </c>
+      <c r="C213" t="s">
+        <v>7</v>
+      </c>
+      <c r="D213" t="s">
+        <v>97</v>
+      </c>
+      <c r="E213" t="s">
+        <v>279</v>
+      </c>
+      <c r="F213">
+        <v>93</v>
+      </c>
+      <c r="J213">
+        <f>SUM(G213, H213,I213)</f>
+        <v>0</v>
+      </c>
+      <c r="K213" t="e">
+        <f>F213/J213</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>94</v>
+      </c>
+      <c r="B214" t="s">
+        <v>81</v>
+      </c>
+      <c r="C214" t="s">
+        <v>7</v>
+      </c>
+      <c r="D214" t="s">
+        <v>97</v>
+      </c>
+      <c r="E214" t="s">
+        <v>280</v>
+      </c>
+      <c r="F214">
+        <v>62</v>
+      </c>
+      <c r="K214" t="e">
+        <f>#REF!/J214</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>94</v>
+      </c>
+      <c r="B215" t="s">
+        <v>81</v>
+      </c>
+      <c r="C215" t="s">
+        <v>7</v>
+      </c>
+      <c r="D215" t="s">
+        <v>97</v>
+      </c>
+      <c r="E215" t="s">
+        <v>281</v>
+      </c>
+      <c r="F215">
+        <v>92</v>
+      </c>
+      <c r="J215">
+        <f>SUM(G215, H215,I215)</f>
+        <v>0</v>
+      </c>
+      <c r="K215" t="e">
+        <f>F215/J215</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>94</v>
+      </c>
+      <c r="B216" t="s">
+        <v>81</v>
+      </c>
+      <c r="C216" t="s">
+        <v>7</v>
+      </c>
+      <c r="D216" t="s">
+        <v>98</v>
+      </c>
+      <c r="E216" t="s">
+        <v>268</v>
+      </c>
+      <c r="F216">
+        <v>71</v>
+      </c>
+      <c r="J216">
+        <f>SUM(G216, H216,I216)</f>
+        <v>0</v>
+      </c>
+      <c r="K216" t="e">
+        <f>F216/J216</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>94</v>
+      </c>
+      <c r="B217" t="s">
+        <v>81</v>
+      </c>
+      <c r="C217" t="s">
+        <v>7</v>
+      </c>
+      <c r="D217" t="s">
+        <v>98</v>
+      </c>
+      <c r="E217" t="s">
+        <v>269</v>
+      </c>
+      <c r="F217">
+        <v>23</v>
+      </c>
+      <c r="J217">
+        <f>SUM(G217, H217,I217)</f>
+        <v>0</v>
+      </c>
+      <c r="K217" t="e">
+        <f>F217/J217</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>94</v>
+      </c>
+      <c r="B218" t="s">
+        <v>81</v>
+      </c>
+      <c r="C218" t="s">
+        <v>7</v>
+      </c>
+      <c r="D218" t="s">
+        <v>98</v>
+      </c>
+      <c r="E218" t="s">
+        <v>270</v>
+      </c>
+      <c r="F218">
+        <v>23</v>
+      </c>
+      <c r="J218">
+        <f>SUM(G218, H218,I218)</f>
+        <v>0</v>
+      </c>
+      <c r="K218" t="e">
+        <f>F218/J218</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>94</v>
+      </c>
+      <c r="B219" t="s">
+        <v>81</v>
+      </c>
+      <c r="C219" t="s">
+        <v>7</v>
+      </c>
+      <c r="D219" t="s">
+        <v>99</v>
+      </c>
+      <c r="E219" t="s">
+        <v>277</v>
+      </c>
+      <c r="F219">
+        <v>96</v>
+      </c>
+      <c r="J219">
+        <f>SUM(G219, H219,I219)</f>
+        <v>0</v>
+      </c>
+      <c r="K219" t="e">
+        <f>F219/J219</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>94</v>
+      </c>
+      <c r="B220" t="s">
+        <v>81</v>
+      </c>
+      <c r="C220" t="s">
+        <v>7</v>
+      </c>
+      <c r="D220" t="s">
+        <v>99</v>
+      </c>
+      <c r="E220" t="s">
+        <v>282</v>
+      </c>
+      <c r="F220">
+        <v>54</v>
+      </c>
+      <c r="J220">
+        <f>SUM(G220, H220,I220)</f>
+        <v>0</v>
+      </c>
+      <c r="K220" t="e">
+        <f>F220/J220</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>94</v>
+      </c>
+      <c r="B221" t="s">
+        <v>81</v>
+      </c>
+      <c r="C221" t="s">
+        <v>7</v>
+      </c>
+      <c r="D221" t="s">
+        <v>99</v>
+      </c>
+      <c r="E221" t="s">
+        <v>272</v>
+      </c>
+      <c r="F221">
+        <v>51</v>
+      </c>
+      <c r="J221">
+        <f>SUM(G221, H221,I221)</f>
+        <v>0</v>
+      </c>
+      <c r="K221" t="e">
+        <f>F221/J221</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>94</v>
+      </c>
+      <c r="B222" t="s">
+        <v>81</v>
+      </c>
+      <c r="C222" t="s">
+        <v>7</v>
+      </c>
+      <c r="D222" t="s">
+        <v>99</v>
+      </c>
+      <c r="E222" t="s">
+        <v>273</v>
+      </c>
+      <c r="F222">
+        <v>53</v>
+      </c>
+      <c r="J222">
+        <f>SUM(G222, H222,I222)</f>
+        <v>0</v>
+      </c>
+      <c r="K222" t="e">
+        <f>F222/J222</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>94</v>
+      </c>
+      <c r="B223" t="s">
+        <v>81</v>
+      </c>
+      <c r="C223" t="s">
+        <v>7</v>
+      </c>
+      <c r="D223" t="s">
+        <v>99</v>
+      </c>
+      <c r="E223" t="s">
+        <v>274</v>
+      </c>
+      <c r="F223">
+        <v>34</v>
+      </c>
+      <c r="J223">
+        <f>SUM(G223, H223,I223)</f>
+        <v>0</v>
+      </c>
+      <c r="K223" t="e">
+        <f>F223/J223</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>94</v>
+      </c>
+      <c r="B224" t="s">
+        <v>81</v>
+      </c>
+      <c r="C224" t="s">
+        <v>7</v>
+      </c>
+      <c r="D224" t="s">
+        <v>99</v>
+      </c>
+      <c r="E224" t="s">
+        <v>275</v>
+      </c>
+      <c r="F224">
+        <v>47</v>
+      </c>
+      <c r="J224">
+        <f>SUM(G224, H224,I224)</f>
+        <v>0</v>
+      </c>
+      <c r="K224" t="e">
+        <f>F224/J224</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>94</v>
+      </c>
+      <c r="B225" t="s">
+        <v>81</v>
+      </c>
+      <c r="C225" t="s">
+        <v>7</v>
+      </c>
+      <c r="D225" t="s">
+        <v>99</v>
+      </c>
+      <c r="E225" t="s">
+        <v>276</v>
+      </c>
+      <c r="F225">
+        <v>6</v>
+      </c>
+      <c r="J225">
+        <f>SUM(G225, H225,I225)</f>
+        <v>0</v>
+      </c>
+      <c r="K225" t="e">
+        <f>F225/J225</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>94</v>
+      </c>
+      <c r="B226" t="s">
+        <v>81</v>
+      </c>
+      <c r="C226" t="s">
+        <v>8</v>
+      </c>
+      <c r="D226" t="s">
+        <v>97</v>
+      </c>
+      <c r="E226" t="s">
+        <v>278</v>
+      </c>
+      <c r="F226">
+        <v>60</v>
+      </c>
+      <c r="J226">
+        <f>SUM(G226, H226,I226)</f>
+        <v>0</v>
+      </c>
+      <c r="K226" t="e">
+        <f>F226/J226</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>94</v>
+      </c>
+      <c r="B227" t="s">
+        <v>81</v>
+      </c>
+      <c r="C227" t="s">
+        <v>8</v>
+      </c>
+      <c r="D227" t="s">
+        <v>97</v>
+      </c>
+      <c r="E227" t="s">
+        <v>279</v>
+      </c>
+      <c r="F227">
+        <v>30</v>
+      </c>
+      <c r="J227">
+        <f>SUM(G227, H227,I227)</f>
+        <v>0</v>
+      </c>
+      <c r="K227" t="e">
+        <f>F227/J227</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>94</v>
+      </c>
+      <c r="B228" t="s">
+        <v>81</v>
+      </c>
+      <c r="C228" t="s">
+        <v>8</v>
+      </c>
+      <c r="D228" t="s">
+        <v>97</v>
+      </c>
+      <c r="E228" t="s">
+        <v>280</v>
+      </c>
+      <c r="F228">
+        <v>60</v>
+      </c>
+      <c r="J228">
+        <f>SUM(G228, H228,I228)</f>
+        <v>0</v>
+      </c>
+      <c r="K228" t="e">
+        <f>F228/J228</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>94</v>
+      </c>
+      <c r="B229" t="s">
+        <v>81</v>
+      </c>
+      <c r="C229" t="s">
+        <v>8</v>
+      </c>
+      <c r="D229" t="s">
+        <v>97</v>
+      </c>
+      <c r="E229" t="s">
+        <v>281</v>
+      </c>
+      <c r="F229">
+        <v>45</v>
+      </c>
+      <c r="J229">
+        <f>SUM(G229, H229,I229)</f>
+        <v>0</v>
+      </c>
+      <c r="K229" t="e">
+        <f>F229/J229</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>94</v>
+      </c>
+      <c r="B230" t="s">
+        <v>81</v>
+      </c>
+      <c r="C230" t="s">
+        <v>8</v>
+      </c>
+      <c r="D230" t="s">
+        <v>99</v>
+      </c>
+      <c r="E230" t="s">
+        <v>271</v>
+      </c>
+      <c r="F230">
+        <v>42</v>
+      </c>
+      <c r="J230">
+        <f>SUM(G230, H230,I230)</f>
+        <v>0</v>
+      </c>
+      <c r="K230" t="e">
+        <f>F230/J230</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>94</v>
+      </c>
+      <c r="B231" t="s">
+        <v>81</v>
+      </c>
+      <c r="C231" t="s">
+        <v>8</v>
+      </c>
+      <c r="D231" t="s">
+        <v>99</v>
+      </c>
+      <c r="E231" t="s">
+        <v>282</v>
+      </c>
+      <c r="F231">
+        <v>33</v>
+      </c>
+      <c r="J231">
+        <f>SUM(G231, H231,I231)</f>
+        <v>0</v>
+      </c>
+      <c r="K231" t="e">
+        <f>F231/J231</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>94</v>
+      </c>
+      <c r="B232" t="s">
+        <v>81</v>
+      </c>
+      <c r="C232" t="s">
+        <v>8</v>
+      </c>
+      <c r="D232" t="s">
+        <v>99</v>
+      </c>
+      <c r="E232" t="s">
+        <v>272</v>
+      </c>
+      <c r="F232">
+        <v>34</v>
+      </c>
+      <c r="J232">
+        <f>SUM(G232, H232,I232)</f>
+        <v>0</v>
+      </c>
+      <c r="K232" t="e">
+        <f>F232/J232</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>94</v>
+      </c>
+      <c r="B233" t="s">
+        <v>81</v>
+      </c>
+      <c r="C233" t="s">
+        <v>8</v>
+      </c>
+      <c r="D233" t="s">
+        <v>99</v>
+      </c>
+      <c r="E233" t="s">
+        <v>273</v>
+      </c>
+      <c r="F233">
+        <v>17</v>
+      </c>
+      <c r="J233">
+        <f>SUM(G233, H233,I233)</f>
+        <v>0</v>
+      </c>
+      <c r="K233" t="e">
+        <f>F233/J233</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>94</v>
+      </c>
+      <c r="B234" t="s">
+        <v>81</v>
+      </c>
+      <c r="C234" t="s">
+        <v>8</v>
+      </c>
+      <c r="D234" t="s">
+        <v>99</v>
+      </c>
+      <c r="E234" t="s">
+        <v>274</v>
+      </c>
+      <c r="F234">
+        <v>34</v>
+      </c>
+      <c r="J234">
+        <f>SUM(G234, H234,I234)</f>
+        <v>0</v>
+      </c>
+      <c r="K234" t="e">
+        <f>F234/J234</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>94</v>
+      </c>
+      <c r="B235" t="s">
+        <v>81</v>
+      </c>
+      <c r="C235" t="s">
+        <v>8</v>
+      </c>
+      <c r="D235" t="s">
+        <v>99</v>
+      </c>
+      <c r="E235" t="s">
+        <v>275</v>
+      </c>
+      <c r="F235">
+        <v>15</v>
+      </c>
+      <c r="J235">
+        <f>SUM(G235, H235,I235)</f>
+        <v>0</v>
+      </c>
+      <c r="K235" t="e">
+        <f>F235/J235</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>94</v>
+      </c>
+      <c r="B236" t="s">
+        <v>81</v>
+      </c>
+      <c r="C236" t="s">
+        <v>8</v>
+      </c>
+      <c r="D236" t="s">
+        <v>99</v>
+      </c>
+      <c r="E236" t="s">
+        <v>276</v>
+      </c>
+      <c r="F236">
+        <v>28</v>
+      </c>
+      <c r="J236">
+        <f>SUM(G236, H236,I236)</f>
+        <v>0</v>
+      </c>
+      <c r="K236" t="e">
+        <f>F236/J236</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M237" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -6889,10 +9696,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6906,7 +9713,7 @@
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6929,7 +9736,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6945,8 +9752,14 @@
       <c r="E2">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>17</v>
       </c>
@@ -6954,7 +9767,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>231</v>
       </c>
@@ -6965,7 +9778,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -6976,7 +9789,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>17</v>
       </c>
@@ -6984,7 +9797,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>231</v>
       </c>
@@ -6995,7 +9808,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>17</v>
       </c>
@@ -7009,7 +9822,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>17</v>
       </c>
@@ -7023,7 +9836,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
@@ -7039,7 +9852,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
@@ -7055,7 +9868,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>10</v>
       </c>
@@ -7069,7 +9882,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>10</v>
       </c>
@@ -7083,7 +9896,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>10</v>
       </c>
@@ -7097,7 +9910,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>10</v>
       </c>
@@ -7111,7 +9924,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
@@ -7524,10 +10337,489 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>231</v>
+      </c>
+      <c r="E48">
+        <v>713</v>
+      </c>
+      <c r="F48">
+        <v>2894</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49">
+        <v>114</v>
+      </c>
+      <c r="F49">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50">
+        <v>95</v>
+      </c>
+      <c r="F50">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>231</v>
+      </c>
+      <c r="E51">
+        <f>SUM(E49,E50)</f>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
+      <c r="E53">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>231</v>
+      </c>
+      <c r="E54">
+        <v>723</v>
+      </c>
+      <c r="F54">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55">
+        <v>170</v>
+      </c>
+      <c r="F55">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E56" s="6">
+        <f>SUM(E46,E49,E52,E55)</f>
+        <v>801</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E57" s="6">
+        <f>SUM(E47,E50,E53)</f>
+        <v>1014</v>
+      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>231</v>
+      </c>
+      <c r="E60">
+        <v>218</v>
+      </c>
+      <c r="F60">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>88</v>
+      </c>
+      <c r="E62">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>231</v>
+      </c>
+      <c r="E63">
+        <v>766</v>
+      </c>
+      <c r="F63">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>88</v>
+      </c>
+      <c r="E65">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>231</v>
+      </c>
+      <c r="E66">
+        <v>619</v>
+      </c>
+      <c r="F66">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E67" s="6">
+        <f>SUM(E58,E61,E64)</f>
+        <v>1179</v>
+      </c>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E68" s="6">
+        <f>SUM(E59,E62,E65)</f>
+        <v>424</v>
+      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>92</v>
+      </c>
+      <c r="E70">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>231</v>
+      </c>
+      <c r="E71">
+        <v>306</v>
+      </c>
+      <c r="F71">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>91</v>
+      </c>
+      <c r="D72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>92</v>
+      </c>
+      <c r="E73">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>231</v>
+      </c>
+      <c r="E74">
+        <v>332</v>
+      </c>
+      <c r="F74">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E75" s="6">
+        <f>SUM(E69,E72)</f>
+        <v>319</v>
+      </c>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E76" s="6">
+        <f>SUM(E70,E73)</f>
+        <v>319</v>
+      </c>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" t="s">
+        <v>98</v>
+      </c>
+      <c r="D77" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>231</v>
+      </c>
+      <c r="E79">
+        <v>869</v>
+      </c>
+      <c r="F79">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>98</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>231</v>
+      </c>
+      <c r="E82">
+        <v>174</v>
+      </c>
+      <c r="F82">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>97</v>
+      </c>
+      <c r="D83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>231</v>
+      </c>
+      <c r="E86">
+        <v>753</v>
+      </c>
+      <c r="F86">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>97</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>231</v>
+      </c>
+      <c r="E89">
+        <v>398</v>
+      </c>
+      <c r="F89">
+        <v>823</v>
+      </c>
+      <c r="G89" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7655,8 +10947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D10"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8871,7 +12163,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>